<commit_message>
Update solution for CP4.2
Add new VOI formulation description.
Add new VOI data (currently produces better results for case 1)
Add note about output columns.
Add clarifications on metrics and submission.
</commit_message>
<xml_diff>
--- a/solutions/problem2/problem-2-solution-voi.xlsx
+++ b/solutions/problem2/problem-2-solution-voi.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin-slater\gh\ppaml-cp4\solutions\problem2\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="16275" windowHeight="7230"/>
+    <workbookView xWindow="120" yWindow="96" windowWidth="16272" windowHeight="7236"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1037,6 +1042,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1084,7 +1092,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1119,7 +1127,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1330,17 +1338,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E153"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="2" customWidth="1"/>
-    <col min="2" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="10.88671875" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1351,7 +1357,7 @@
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -1366,41 +1372,41 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2">
-        <v>-3.8275999999999999</v>
+        <v>-110.31516426844399</v>
       </c>
       <c r="C3" s="2">
         <v>0</v>
       </c>
       <c r="D3" s="2">
-        <v>-3.8275999999999999</v>
+        <v>-1848.1753687029</v>
       </c>
       <c r="E3" s="2">
-        <v>-3.8275999999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1665.35668249536</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="2">
-        <v>-4.5431999999999997</v>
+        <v>-112.994959703234</v>
       </c>
       <c r="C4" s="2">
-        <v>-4.5431999999999997</v>
+        <v>-903.79563969236494</v>
       </c>
       <c r="D4" s="2">
-        <v>-4.5431999999999997</v>
+        <v>-1324.4890770602799</v>
       </c>
       <c r="E4" s="2">
-        <v>-4.5431999999999997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1789.41519615985</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1408,50 +1414,50 @@
         <v>0</v>
       </c>
       <c r="C5" s="2">
-        <v>-2.3580000000000001</v>
+        <v>-958.55303776867402</v>
       </c>
       <c r="D5" s="2">
-        <v>-2.3580000000000001</v>
+        <v>-1827.11824411875</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="2">
-        <v>-3.2507000000000001</v>
+        <v>-26.230830025593601</v>
       </c>
       <c r="C6" s="2">
-        <v>-3.2507000000000001</v>
+        <v>-934.81557855563199</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
       </c>
       <c r="E6" s="2">
-        <v>-3.2507000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1629.0417332685799</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="2">
-        <v>-5.0648999999999997</v>
+        <v>-18.4370378088088</v>
       </c>
       <c r="C7" s="2">
-        <v>-5.0648999999999997</v>
+        <v>-958.49144594745405</v>
       </c>
       <c r="D7" s="2">
-        <v>-5.0648999999999997</v>
+        <v>-1821.39340573923</v>
       </c>
       <c r="E7" s="2">
-        <v>-5.0648999999999997</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1712.04276010334</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1459,7 +1465,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="2">
-        <v>-2.0587</v>
+        <v>-870.01396242122701</v>
       </c>
       <c r="D8" s="2">
         <v>0</v>
@@ -1468,7 +1474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1479,98 +1485,98 @@
         <v>0</v>
       </c>
       <c r="D9" s="2">
-        <v>-2.9516</v>
+        <v>-1588.48969505642</v>
       </c>
       <c r="E9" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="2">
-        <v>-3.8561999999999999</v>
+        <v>-162.57388545734699</v>
       </c>
       <c r="C10" s="2">
-        <v>-3.8561999999999999</v>
+        <v>-954.98323603708297</v>
       </c>
       <c r="D10" s="2">
-        <v>-3.8561999999999999</v>
+        <v>-1801.83980452623</v>
       </c>
       <c r="E10" s="2">
-        <v>-3.8561999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1694.82386934489</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="2">
-        <v>-7.6002000000000001</v>
+        <v>19.581024875347101</v>
       </c>
       <c r="C11" s="2">
-        <v>-7.6002000000000001</v>
+        <v>-782.94856629690003</v>
       </c>
       <c r="D11" s="2">
-        <v>-7.6002000000000001</v>
+        <v>-1634.1332619858999</v>
       </c>
       <c r="E11" s="2">
-        <v>-7.6002000000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1680.1148162305501</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="2">
-        <v>-8.2105999999999995</v>
+        <v>13.634870629455101</v>
       </c>
       <c r="C12" s="2">
-        <v>-8.2105999999999995</v>
+        <v>-896.98189281574298</v>
       </c>
       <c r="D12" s="2">
-        <v>-8.2105999999999995</v>
+        <v>-1791.40428846226</v>
       </c>
       <c r="E12" s="2">
-        <v>-8.2105999999999995</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1683.18638635506</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="2">
-        <v>-3.6347999999999998</v>
+        <v>-39.559889176117203</v>
       </c>
       <c r="C13" s="2">
-        <v>-3.6347999999999998</v>
+        <v>-723.88291732329196</v>
       </c>
       <c r="D13" s="2">
-        <v>-3.6347999999999998</v>
+        <v>-1534.5464094378201</v>
       </c>
       <c r="E13" s="2">
-        <v>-3.6347999999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1634.7913646135601</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="2">
-        <v>-5.0702999999999996</v>
+        <v>-67.375854871904707</v>
       </c>
       <c r="C14" s="2">
-        <v>-5.0702999999999996</v>
+        <v>-928.36788629660998</v>
       </c>
       <c r="D14" s="2">
-        <v>-5.0702999999999996</v>
+        <v>-1831.3429981854299</v>
       </c>
       <c r="E14" s="2">
-        <v>-5.0702999999999996</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1698.0873769398099</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
@@ -1578,50 +1584,50 @@
         <v>0</v>
       </c>
       <c r="C15" s="2">
-        <v>-7.5136000000000003</v>
+        <v>-589.26960549022499</v>
       </c>
       <c r="D15" s="2">
-        <v>-7.5136000000000003</v>
+        <v>-1786.1173105811399</v>
       </c>
       <c r="E15" s="2">
-        <v>-7.5136000000000003</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1633.03607839652</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="2">
-        <v>-7.6148999999999996</v>
+        <v>-3.01786206799602</v>
       </c>
       <c r="C16" s="2">
-        <v>-7.6148999999999996</v>
+        <v>-680.32035426247705</v>
       </c>
       <c r="D16" s="2">
-        <v>-7.6148999999999996</v>
+        <v>-1565.09059022613</v>
       </c>
       <c r="E16" s="2">
-        <v>-7.6148999999999996</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1677.7524909891599</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="2">
-        <v>-4.4458000000000002</v>
+        <v>-77.534444352913695</v>
       </c>
       <c r="C17" s="2">
-        <v>-4.4458000000000002</v>
+        <v>-961.08503079324498</v>
       </c>
       <c r="D17" s="2">
-        <v>-4.4458000000000002</v>
+        <v>-1775.2344439093499</v>
       </c>
       <c r="E17" s="2">
-        <v>-4.4458000000000002</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1627.1184861418601</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
@@ -1632,13 +1638,13 @@
         <v>0</v>
       </c>
       <c r="D18" s="2">
-        <v>-3.2637999999999998</v>
+        <v>-1806.58077662084</v>
       </c>
       <c r="E18" s="2">
-        <v>-3.2637999999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1712.46838766105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
@@ -1652,44 +1658,44 @@
         <v>0</v>
       </c>
       <c r="E19" s="2">
-        <v>-3.5442999999999998</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1707.9824767733601</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B20" s="2">
-        <v>-4.6914999999999996</v>
+        <v>-54.938361870946899</v>
       </c>
       <c r="C20" s="2">
-        <v>-4.6914999999999996</v>
+        <v>-859.93028094261297</v>
       </c>
       <c r="D20" s="2">
         <v>0</v>
       </c>
       <c r="E20" s="2">
-        <v>-4.6914999999999996</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1671.9188469196999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B21" s="2">
-        <v>-10.051600000000001</v>
+        <v>-38.131097966687499</v>
       </c>
       <c r="C21" s="2">
-        <v>-10.051600000000001</v>
+        <v>-946.42296303884996</v>
       </c>
       <c r="D21" s="2">
-        <v>-10.051600000000001</v>
+        <v>-1790.8550584597299</v>
       </c>
       <c r="E21" s="2">
-        <v>-10.051600000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1676.6280650315</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>25</v>
       </c>
@@ -1697,16 +1703,16 @@
         <v>0</v>
       </c>
       <c r="C22" s="2">
-        <v>-4.2531999999999996</v>
+        <v>-948.60657604286803</v>
       </c>
       <c r="D22" s="2">
-        <v>-4.2531999999999996</v>
+        <v>-1737.55493226261</v>
       </c>
       <c r="E22" s="2">
-        <v>-4.2531999999999996</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1672.8874354223501</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
@@ -1723,29 +1729,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="2">
-        <v>-7.0481999999999996</v>
+        <v>-57.294920939978098</v>
       </c>
       <c r="C24" s="2">
-        <v>-7.0481999999999996</v>
+        <v>-952.41103531937995</v>
       </c>
       <c r="D24" s="2">
-        <v>-7.0481999999999996</v>
+        <v>-1752.8420326078301</v>
       </c>
       <c r="E24" s="2">
-        <v>-7.0481999999999996</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1533.3587450799901</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B25" s="2">
-        <v>-3.6637</v>
+        <v>31.1798421792375</v>
       </c>
       <c r="C25" s="2">
         <v>0</v>
@@ -1757,63 +1763,63 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B26" s="2">
-        <v>-3.2847</v>
+        <v>13.857312611223101</v>
       </c>
       <c r="C26" s="2">
-        <v>-3.2847</v>
+        <v>-690.97070768811795</v>
       </c>
       <c r="D26" s="2">
-        <v>-3.2847</v>
+        <v>-1806.37335417194</v>
       </c>
       <c r="E26" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B27" s="2">
-        <v>-9.0805000000000007</v>
+        <v>-97.653596985239901</v>
       </c>
       <c r="C27" s="2">
-        <v>-9.0805000000000007</v>
+        <v>-973.78058160717501</v>
       </c>
       <c r="D27" s="2">
-        <v>-9.0805000000000007</v>
+        <v>-1487.3962418485301</v>
       </c>
       <c r="E27" s="2">
-        <v>-9.0805000000000007</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1577.68420325178</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B28" s="2">
-        <v>-6.5586000000000002</v>
+        <v>20.7833485731264</v>
       </c>
       <c r="C28" s="2">
-        <v>-6.5586000000000002</v>
+        <v>-793.515847411256</v>
       </c>
       <c r="D28" s="2">
-        <v>-6.5586000000000002</v>
+        <v>-1508.1976557657099</v>
       </c>
       <c r="E28" s="2">
-        <v>-6.5586000000000002</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1706.96163877709</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B29" s="2">
-        <v>-2.1844000000000001</v>
+        <v>-46.787656013303398</v>
       </c>
       <c r="C29" s="2">
         <v>0</v>
@@ -1825,58 +1831,58 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B30" s="2">
-        <v>-6.4699</v>
+        <v>-40.574524052293</v>
       </c>
       <c r="C30" s="2">
-        <v>-6.4699</v>
+        <v>-951.18501444453</v>
       </c>
       <c r="D30" s="2">
-        <v>-6.4699</v>
+        <v>-1793.3945657469301</v>
       </c>
       <c r="E30" s="2">
-        <v>-6.4699</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1732.4238255355999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B31" s="2">
-        <v>-5.0651000000000002</v>
+        <v>-33.069148170210802</v>
       </c>
       <c r="C31" s="2">
-        <v>-5.0651000000000002</v>
+        <v>-905.69126349663998</v>
       </c>
       <c r="D31" s="2">
-        <v>-5.0651000000000002</v>
+        <v>-1786.4779429965099</v>
       </c>
       <c r="E31" s="2">
-        <v>-5.0651000000000002</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1618.6541443102001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B32" s="2">
-        <v>-7.2869000000000002</v>
+        <v>0.79457328950628403</v>
       </c>
       <c r="C32" s="2">
-        <v>-7.2869000000000002</v>
+        <v>-954.05893657795696</v>
       </c>
       <c r="D32" s="2">
-        <v>-7.2869000000000002</v>
+        <v>-1814.8559782464399</v>
       </c>
       <c r="E32" s="2">
-        <v>-7.2869000000000002</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1703.52355520624</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>36</v>
       </c>
@@ -1890,256 +1896,256 @@
         <v>0</v>
       </c>
       <c r="E33" s="2">
-        <v>-3.6034999999999999</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1685.2420552266899</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B34" s="2">
-        <v>-4.5895999999999999</v>
+        <v>-44.314399411917201</v>
       </c>
       <c r="C34" s="2">
-        <v>-4.5895999999999999</v>
+        <v>-936.98815637377095</v>
       </c>
       <c r="D34" s="2">
-        <v>-4.5895999999999999</v>
+        <v>-1821.1839162354499</v>
       </c>
       <c r="E34" s="2">
-        <v>-4.5895999999999999</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1583.5085370250599</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B35" s="2">
-        <v>-4.5614999999999997</v>
+        <v>-50.169852465122403</v>
       </c>
       <c r="C35" s="2">
-        <v>-4.5614999999999997</v>
+        <v>-943.08124513084397</v>
       </c>
       <c r="D35" s="2">
-        <v>-4.5614999999999997</v>
+        <v>-1824.38788012693</v>
       </c>
       <c r="E35" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B36" s="2">
-        <v>-4.9484000000000004</v>
+        <v>-69.113180804199104</v>
       </c>
       <c r="C36" s="2">
-        <v>-4.9484000000000004</v>
+        <v>-968.50924135461003</v>
       </c>
       <c r="D36" s="2">
-        <v>-4.9484000000000004</v>
+        <v>-1760.3025662600801</v>
       </c>
       <c r="E36" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B37" s="2">
-        <v>-4.5629</v>
+        <v>-33.376253118115201</v>
       </c>
       <c r="C37" s="2">
         <v>0</v>
       </c>
       <c r="D37" s="2">
-        <v>-4.5629</v>
+        <v>-1768.2301189065099</v>
       </c>
       <c r="E37" s="2">
-        <v>-4.5629</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1674.8046293111299</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B38" s="2">
-        <v>-5.8966000000000003</v>
+        <v>-17.093136446910201</v>
       </c>
       <c r="C38" s="2">
-        <v>-5.8966000000000003</v>
+        <v>-941.30019204917198</v>
       </c>
       <c r="D38" s="2">
-        <v>-5.8966000000000003</v>
+        <v>-1756.09920918021</v>
       </c>
       <c r="E38" s="2">
-        <v>-5.8966000000000003</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1675.1687736687099</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B39" s="2">
-        <v>-5.1167999999999996</v>
+        <v>31.023390190440999</v>
       </c>
       <c r="C39" s="2">
-        <v>-5.1167999999999996</v>
+        <v>-954.50917490959796</v>
       </c>
       <c r="D39" s="2">
-        <v>-5.1167999999999996</v>
+        <v>-1737.21089482447</v>
       </c>
       <c r="E39" s="2">
-        <v>-5.1167999999999996</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1661.6909357494901</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B40" s="2">
-        <v>-4.8209</v>
+        <v>-0.71975320167780399</v>
       </c>
       <c r="C40" s="2">
         <v>0</v>
       </c>
       <c r="D40" s="2">
-        <v>-4.8209</v>
+        <v>-1713.53982897264</v>
       </c>
       <c r="E40" s="2">
-        <v>-4.8209</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1677.49423205978</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B41" s="2">
-        <v>-7.4333999999999998</v>
+        <v>4.9347099462102104</v>
       </c>
       <c r="C41" s="2">
-        <v>-7.4333999999999998</v>
+        <v>-589.61777350605598</v>
       </c>
       <c r="D41" s="2">
-        <v>-7.4333999999999998</v>
+        <v>-1378.8848079505501</v>
       </c>
       <c r="E41" s="2">
-        <v>-7.4333999999999998</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1708.15259390039</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B42" s="2">
-        <v>-4.9185999999999996</v>
+        <v>12.3457771781601</v>
       </c>
       <c r="C42" s="2">
-        <v>-4.9185999999999996</v>
+        <v>-964.48529324014203</v>
       </c>
       <c r="D42" s="2">
-        <v>-4.9185999999999996</v>
+        <v>-1757.0664679338399</v>
       </c>
       <c r="E42" s="2">
-        <v>-4.9185999999999996</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1665.97654643838</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B43" s="2">
-        <v>-6.3944999999999999</v>
+        <v>-33.322588440724303</v>
       </c>
       <c r="C43" s="2">
-        <v>-6.3944999999999999</v>
+        <v>-915.52592885690399</v>
       </c>
       <c r="D43" s="2">
-        <v>-6.3944999999999999</v>
+        <v>-1724.56574652932</v>
       </c>
       <c r="E43" s="2">
-        <v>-6.3944999999999999</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1566.82486529167</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B44" s="2">
-        <v>-7.8285</v>
+        <v>-46.748300822020198</v>
       </c>
       <c r="C44" s="2">
-        <v>-7.8285</v>
+        <v>-833.33859393265595</v>
       </c>
       <c r="D44" s="2">
-        <v>-7.8285</v>
+        <v>-1752.8203380116399</v>
       </c>
       <c r="E44" s="2">
-        <v>-7.8285</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1672.7494666477401</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B45" s="2">
-        <v>-7.1280000000000001</v>
+        <v>-73.651771942259302</v>
       </c>
       <c r="C45" s="2">
-        <v>-7.1280000000000001</v>
+        <v>-961.49807184222902</v>
       </c>
       <c r="D45" s="2">
-        <v>-7.1280000000000001</v>
+        <v>-1825.9709002030199</v>
       </c>
       <c r="E45" s="2">
-        <v>-7.1280000000000001</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1697.1008658763401</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B46" s="2">
-        <v>-6.1980000000000004</v>
+        <v>-4.2903717082276698</v>
       </c>
       <c r="C46" s="2">
-        <v>-6.1980000000000004</v>
+        <v>-635.651347745002</v>
       </c>
       <c r="D46" s="2">
-        <v>-6.1980000000000004</v>
+        <v>-1594.6549575036299</v>
       </c>
       <c r="E46" s="2">
-        <v>-6.1980000000000004</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1691.4382373481999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B47" s="2">
-        <v>-4.9340000000000002</v>
+        <v>-78.661532492984605</v>
       </c>
       <c r="C47" s="2">
-        <v>-4.9340000000000002</v>
+        <v>-971.993374861181</v>
       </c>
       <c r="D47" s="2">
-        <v>-4.9340000000000002</v>
+        <v>-1805.97012506497</v>
       </c>
       <c r="E47" s="2">
-        <v>-4.9340000000000002</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1637.32605754774</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B48" s="2">
-        <v>-3.1566000000000001</v>
+        <v>-122.201885476199</v>
       </c>
       <c r="C48" s="2">
-        <v>-3.1566000000000001</v>
+        <v>-944.51523927619803</v>
       </c>
       <c r="D48" s="2">
         <v>0</v>
@@ -2148,75 +2154,75 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B49" s="2">
-        <v>-4.5199999999999996</v>
+        <v>2.81640493950461</v>
       </c>
       <c r="C49" s="2">
-        <v>-4.5199999999999996</v>
+        <v>-952.07182219689605</v>
       </c>
       <c r="D49" s="2">
-        <v>-4.5199999999999996</v>
+        <v>-1595.3493537193101</v>
       </c>
       <c r="E49" s="2">
-        <v>-4.5199999999999996</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1494.18232069345</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B50" s="2">
-        <v>-5.9497</v>
+        <v>-23.3884302464519</v>
       </c>
       <c r="C50" s="2">
-        <v>-5.9497</v>
+        <v>-916.85135410355304</v>
       </c>
       <c r="D50" s="2">
-        <v>-5.9497</v>
+        <v>-1804.96564978387</v>
       </c>
       <c r="E50" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B51" s="2">
-        <v>-7.4352</v>
+        <v>14.144686245712601</v>
       </c>
       <c r="C51" s="2">
-        <v>-7.4352</v>
+        <v>-965.41188262732203</v>
       </c>
       <c r="D51" s="2">
-        <v>-7.4352</v>
+        <v>-1822.5958525916501</v>
       </c>
       <c r="E51" s="2">
-        <v>-7.4352</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1476.75163059796</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B52" s="2">
-        <v>-6.4745999999999997</v>
+        <v>-105.65103978125001</v>
       </c>
       <c r="C52" s="2">
-        <v>-6.4745999999999997</v>
+        <v>-958.57844905915499</v>
       </c>
       <c r="D52" s="2">
-        <v>-6.4745999999999997</v>
+        <v>-1811.20755985085</v>
       </c>
       <c r="E52" s="2">
-        <v>-6.4745999999999997</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1632.45991435172</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>56</v>
       </c>
@@ -2224,33 +2230,33 @@
         <v>0</v>
       </c>
       <c r="C53" s="2">
-        <v>-3.5586000000000002</v>
+        <v>-894.26703954127299</v>
       </c>
       <c r="D53" s="2">
-        <v>-3.5586000000000002</v>
+        <v>-1795.31193427075</v>
       </c>
       <c r="E53" s="2">
-        <v>-3.5586000000000002</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1680.21534989474</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B54" s="2">
-        <v>-5.9870000000000001</v>
+        <v>13.676569062275</v>
       </c>
       <c r="C54" s="2">
-        <v>-5.9870000000000001</v>
+        <v>-937.32214279200196</v>
       </c>
       <c r="D54" s="2">
-        <v>-5.9870000000000001</v>
+        <v>-1655.62936608672</v>
       </c>
       <c r="E54" s="2">
-        <v>-5.9870000000000001</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1547.12656800888</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>58</v>
       </c>
@@ -2261,81 +2267,81 @@
         <v>0</v>
       </c>
       <c r="D55" s="2">
-        <v>-3.0949</v>
+        <v>-1805.9951414689299</v>
       </c>
       <c r="E55" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B56" s="2">
-        <v>-4.7754000000000003</v>
+        <v>-78.154968696770496</v>
       </c>
       <c r="C56" s="2">
-        <v>-4.7754000000000003</v>
+        <v>-983.24918522522898</v>
       </c>
       <c r="D56" s="2">
-        <v>-4.7754000000000003</v>
+        <v>-1844.06245075329</v>
       </c>
       <c r="E56" s="2">
-        <v>-4.7754000000000003</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1658.3618521303699</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B57" s="2">
-        <v>-4.1864999999999997</v>
+        <v>-75.306583961309101</v>
       </c>
       <c r="C57" s="2">
-        <v>-4.1864999999999997</v>
+        <v>-975.01072467731103</v>
       </c>
       <c r="D57" s="2">
-        <v>-4.1864999999999997</v>
+        <v>-1821.0760378397099</v>
       </c>
       <c r="E57" s="2">
-        <v>-4.1864999999999997</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1687.28455529024</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B58" s="2">
-        <v>-3.7090999999999998</v>
+        <v>-20.416469959506099</v>
       </c>
       <c r="C58" s="2">
         <v>0</v>
       </c>
       <c r="D58" s="2">
-        <v>-3.7090999999999998</v>
+        <v>-1694.8331927663</v>
       </c>
       <c r="E58" s="2">
-        <v>-3.7090999999999998</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1594.8883787925599</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B59" s="2">
-        <v>-4.8045</v>
+        <v>-34.179042792687298</v>
       </c>
       <c r="C59" s="2">
-        <v>-4.8045</v>
+        <v>-959.93053868248001</v>
       </c>
       <c r="D59" s="2">
-        <v>-4.8045</v>
+        <v>-1779.95179380273</v>
       </c>
       <c r="E59" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>63</v>
       </c>
@@ -2346,55 +2352,55 @@
         <v>0</v>
       </c>
       <c r="D60" s="2">
-        <v>-4.0168999999999997</v>
+        <v>-1469.50647785298</v>
       </c>
       <c r="E60" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B61" s="2">
-        <v>-5.1113999999999997</v>
+        <v>-33.550877297761403</v>
       </c>
       <c r="C61" s="2">
-        <v>-5.1113999999999997</v>
+        <v>-967.02527296791197</v>
       </c>
       <c r="D61" s="2">
-        <v>-5.1113999999999997</v>
+        <v>-1821.1480174114199</v>
       </c>
       <c r="E61" s="2">
-        <v>-5.1113999999999997</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1541.0395190315101</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B62" s="2">
-        <v>-4.5766</v>
+        <v>-68.003611556546801</v>
       </c>
       <c r="C62" s="2">
-        <v>-4.5766</v>
+        <v>-968.35674489119401</v>
       </c>
       <c r="D62" s="2">
-        <v>-4.5766</v>
+        <v>-1766.2588592429299</v>
       </c>
       <c r="E62" s="2">
-        <v>-4.5766</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1633.9886774054301</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B63" s="2">
-        <v>-3.8792</v>
+        <v>-56.8516381981824</v>
       </c>
       <c r="C63" s="2">
-        <v>-3.8792</v>
+        <v>-955.10733170851495</v>
       </c>
       <c r="D63" s="2">
         <v>0</v>
@@ -2403,29 +2409,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B64" s="2">
-        <v>-4.3903999999999996</v>
+        <v>-80.506657591110198</v>
       </c>
       <c r="C64" s="2">
-        <v>-4.3903999999999996</v>
+        <v>-896.34893274513195</v>
       </c>
       <c r="D64" s="2">
-        <v>-4.3903999999999996</v>
+        <v>-1756.7803616230401</v>
       </c>
       <c r="E64" s="2">
-        <v>-4.3903999999999996</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1616.4395143701699</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B65" s="2">
-        <v>-3.7549999999999999</v>
+        <v>-15.1152027240846</v>
       </c>
       <c r="C65" s="2">
         <v>0</v>
@@ -2434,44 +2440,44 @@
         <v>0</v>
       </c>
       <c r="E65" s="2">
-        <v>-3.7549999999999999</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1667.3960375900499</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B66" s="2">
-        <v>-2.1659000000000002</v>
+        <v>-86.196662521621903</v>
       </c>
       <c r="C66" s="2">
         <v>0</v>
       </c>
       <c r="D66" s="2">
-        <v>-2.1659000000000002</v>
+        <v>-1313.1623829085399</v>
       </c>
       <c r="E66" s="2">
-        <v>-2.1659000000000002</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1725.1750194882</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B67" s="2">
-        <v>-5.0442999999999998</v>
+        <v>-62.528658552305103</v>
       </c>
       <c r="C67" s="2">
-        <v>-5.0442999999999998</v>
+        <v>-923.71807737706604</v>
       </c>
       <c r="D67" s="2">
-        <v>-5.0442999999999998</v>
+        <v>-1851.29730026213</v>
       </c>
       <c r="E67" s="2">
-        <v>-5.0442999999999998</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1576.8296814277101</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>71</v>
       </c>
@@ -2485,61 +2491,61 @@
         <v>0</v>
       </c>
       <c r="E68" s="2">
-        <v>-3.1105999999999998</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1667.31527983007</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B69" s="2">
-        <v>-2.9925000000000002</v>
+        <v>-24.434269579181802</v>
       </c>
       <c r="C69" s="2">
-        <v>-2.9925000000000002</v>
+        <v>-905.41357469328204</v>
       </c>
       <c r="D69" s="2">
-        <v>-2.9925000000000002</v>
+        <v>-1793.2376495405899</v>
       </c>
       <c r="E69" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B70" s="2">
-        <v>-5.8672000000000004</v>
+        <v>4.6972514316478904</v>
       </c>
       <c r="C70" s="2">
-        <v>-5.8672000000000004</v>
+        <v>-899.11467631808205</v>
       </c>
       <c r="D70" s="2">
-        <v>-5.8672000000000004</v>
+        <v>-1770.25563552125</v>
       </c>
       <c r="E70" s="2">
-        <v>-5.8672000000000004</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1676.31437582849</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B71" s="2">
-        <v>-10.972099999999999</v>
+        <v>-216.31670685463999</v>
       </c>
       <c r="C71" s="2">
-        <v>-10.972099999999999</v>
+        <v>-354.20804322057597</v>
       </c>
       <c r="D71" s="2">
-        <v>-10.972099999999999</v>
+        <v>-1282.15991508662</v>
       </c>
       <c r="E71" s="2">
-        <v>-10.972099999999999</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1767.5510558705701</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>75</v>
       </c>
@@ -2547,84 +2553,84 @@
         <v>0</v>
       </c>
       <c r="C72" s="2">
-        <v>-3.7818999999999998</v>
+        <v>-692.33149865597704</v>
       </c>
       <c r="D72" s="2">
-        <v>-3.7818999999999998</v>
+        <v>-1567.23946221079</v>
       </c>
       <c r="E72" s="2">
-        <v>-3.7818999999999998</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1665.70155170975</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B73" s="2">
-        <v>-6.5145999999999997</v>
+        <v>17.269386427410801</v>
       </c>
       <c r="C73" s="2">
-        <v>-6.5145999999999997</v>
+        <v>-868.78688598926306</v>
       </c>
       <c r="D73" s="2">
-        <v>-6.5145999999999997</v>
+        <v>-1689.64686583364</v>
       </c>
       <c r="E73" s="2">
-        <v>-6.5145999999999997</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1675.07011191674</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B74" s="2">
-        <v>-4.4335000000000004</v>
+        <v>21.342849366650199</v>
       </c>
       <c r="C74" s="2">
-        <v>-4.4335000000000004</v>
+        <v>-843.018586562991</v>
       </c>
       <c r="D74" s="2">
-        <v>-4.4335000000000004</v>
+        <v>-1760.02073647527</v>
       </c>
       <c r="E74" s="2">
-        <v>-4.4335000000000004</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1648.8074990943301</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B75" s="2">
-        <v>-5.0350000000000001</v>
+        <v>25.600143398876799</v>
       </c>
       <c r="C75" s="2">
-        <v>-5.0350000000000001</v>
+        <v>-724.59001229306102</v>
       </c>
       <c r="D75" s="2">
-        <v>-5.0350000000000001</v>
+        <v>-1437.5301518024501</v>
       </c>
       <c r="E75" s="2">
-        <v>-5.0350000000000001</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1706.37250735579</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B76" s="2">
-        <v>-8.3873999999999995</v>
+        <v>34.197692143290404</v>
       </c>
       <c r="C76" s="2">
-        <v>-8.3873999999999995</v>
+        <v>-858.083918803507</v>
       </c>
       <c r="D76" s="2">
-        <v>-8.3873999999999995</v>
+        <v>-1470.95893531251</v>
       </c>
       <c r="E76" s="2">
-        <v>-8.3873999999999995</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1588.3483991103799</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>80</v>
       </c>
@@ -2641,58 +2647,58 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B78" s="2">
-        <v>-12.003399999999999</v>
+        <v>-83.809392409176496</v>
       </c>
       <c r="C78" s="2">
-        <v>-12.003399999999999</v>
+        <v>-937.29966186569698</v>
       </c>
       <c r="D78" s="2">
-        <v>-12.003399999999999</v>
+        <v>-1826.45445213165</v>
       </c>
       <c r="E78" s="2">
-        <v>-12.003399999999999</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1683.1263283405699</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B79" s="2">
-        <v>-5.8228999999999997</v>
+        <v>-6.3056196534903401</v>
       </c>
       <c r="C79" s="2">
-        <v>-5.8228999999999997</v>
+        <v>-966.97365648734399</v>
       </c>
       <c r="D79" s="2">
-        <v>-5.8228999999999997</v>
+        <v>-1670.6618218928299</v>
       </c>
       <c r="E79" s="2">
-        <v>-5.8228999999999997</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1642.14332151386</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B80" s="2">
-        <v>-5.6833999999999998</v>
+        <v>50.750733617729402</v>
       </c>
       <c r="C80" s="2">
-        <v>-5.6833999999999998</v>
+        <v>-891.67413035328002</v>
       </c>
       <c r="D80" s="2">
-        <v>-5.6833999999999998</v>
+        <v>-1779.13082771428</v>
       </c>
       <c r="E80" s="2">
-        <v>-5.6833999999999998</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1440.8181994614199</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>84</v>
       </c>
@@ -2700,106 +2706,106 @@
         <v>0</v>
       </c>
       <c r="C81" s="2">
-        <v>-3.5804999999999998</v>
+        <v>-957.62602634297798</v>
       </c>
       <c r="D81" s="2">
-        <v>-3.5804999999999998</v>
+        <v>-1768.2548939542901</v>
       </c>
       <c r="E81" s="2">
-        <v>-3.5804999999999998</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1684.0232878859799</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B82" s="2">
-        <v>-2.9645999999999999</v>
+        <v>-53.244179163678403</v>
       </c>
       <c r="C82" s="2">
-        <v>-2.9645999999999999</v>
+        <v>-939.12133958760603</v>
       </c>
       <c r="D82" s="2">
-        <v>-2.9645999999999999</v>
+        <v>-1766.7051766381101</v>
       </c>
       <c r="E82" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B83" s="2">
-        <v>-5.4246999999999996</v>
+        <v>-4.6293536797933301</v>
       </c>
       <c r="C83" s="2">
-        <v>-5.4246999999999996</v>
+        <v>-910.06980558563998</v>
       </c>
       <c r="D83" s="2">
-        <v>-5.4246999999999996</v>
+        <v>-1778.0795132390399</v>
       </c>
       <c r="E83" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B84" s="2">
-        <v>-7.7270000000000003</v>
+        <v>-11.733310407976299</v>
       </c>
       <c r="C84" s="2">
-        <v>-7.7270000000000003</v>
+        <v>-967.12291210117201</v>
       </c>
       <c r="D84" s="2">
-        <v>-7.7270000000000003</v>
+        <v>-1657.9130139123399</v>
       </c>
       <c r="E84" s="2">
-        <v>-7.7270000000000003</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1681.1720735742899</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B85" s="2">
-        <v>-4.3994999999999997</v>
+        <v>10.991543883670101</v>
       </c>
       <c r="C85" s="2">
-        <v>-4.3994999999999997</v>
+        <v>-869.88311582018605</v>
       </c>
       <c r="D85" s="2">
-        <v>-4.3994999999999997</v>
+        <v>-1644.93061939209</v>
       </c>
       <c r="E85" s="2">
-        <v>-4.3994999999999997</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1690.1034261223101</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B86" s="2">
-        <v>-4.1108000000000002</v>
+        <v>5.0279996531779201</v>
       </c>
       <c r="C86" s="2">
         <v>0</v>
       </c>
       <c r="D86" s="2">
-        <v>-4.1108000000000002</v>
+        <v>-1807.54595895324</v>
       </c>
       <c r="E86" s="2">
-        <v>-4.1108000000000002</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1673.1742935099401</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B87" s="2">
-        <v>-3.0364</v>
+        <v>4.9044898918988098</v>
       </c>
       <c r="C87" s="2">
         <v>0</v>
@@ -2808,78 +2814,78 @@
         <v>0</v>
       </c>
       <c r="E87" s="2">
-        <v>-3.0364</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1563.5825969437001</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B88" s="2">
-        <v>-4.4406999999999996</v>
+        <v>13.4324629687091</v>
       </c>
       <c r="C88" s="2">
-        <v>-4.4406999999999996</v>
+        <v>-953.05154745035099</v>
       </c>
       <c r="D88" s="2">
-        <v>-4.4406999999999996</v>
+        <v>-1475.31975702626</v>
       </c>
       <c r="E88" s="2">
-        <v>-4.4406999999999996</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1577.54048518791</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B89" s="2">
-        <v>-5.2314999999999996</v>
+        <v>-19.963224283254601</v>
       </c>
       <c r="C89" s="2">
-        <v>-5.2314999999999996</v>
+        <v>-962.08626929715194</v>
       </c>
       <c r="D89" s="2">
-        <v>-5.2314999999999996</v>
+        <v>-1784.12091093195</v>
       </c>
       <c r="E89" s="2">
-        <v>-5.2314999999999996</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1644.69619058852</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B90" s="2">
-        <v>-4.3654000000000002</v>
+        <v>-64.929699468283303</v>
       </c>
       <c r="C90" s="2">
-        <v>-4.3654000000000002</v>
+        <v>-959.82585234696899</v>
       </c>
       <c r="D90" s="2">
         <v>0</v>
       </c>
       <c r="E90" s="2">
-        <v>-4.3654000000000002</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1709.1436268441801</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B91" s="2">
-        <v>-4.9249000000000001</v>
+        <v>-49.581932858572898</v>
       </c>
       <c r="C91" s="2">
-        <v>-4.9249000000000001</v>
+        <v>-981.52096418703297</v>
       </c>
       <c r="D91" s="2">
-        <v>-4.9249000000000001</v>
+        <v>-1737.15175157162</v>
       </c>
       <c r="E91" s="2">
-        <v>-4.9249000000000001</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1548.6228800579599</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>95</v>
       </c>
@@ -2893,27 +2899,27 @@
         <v>0</v>
       </c>
       <c r="E92" s="2">
-        <v>-2.476</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1591.1172152207</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>96</v>
       </c>
       <c r="B93" s="2">
-        <v>-6.4997999999999996</v>
+        <v>-21.828198117577401</v>
       </c>
       <c r="C93" s="2">
-        <v>-6.4997999999999996</v>
+        <v>-630.11133161542</v>
       </c>
       <c r="D93" s="2">
         <v>0</v>
       </c>
       <c r="E93" s="2">
-        <v>-6.4997999999999996</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1656.64656523952</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>97</v>
       </c>
@@ -2921,16 +2927,16 @@
         <v>0</v>
       </c>
       <c r="C94" s="2">
-        <v>-2.8500999999999999</v>
+        <v>-872.83722461945695</v>
       </c>
       <c r="D94" s="2">
-        <v>-2.8500999999999999</v>
+        <v>-1809.1796700431901</v>
       </c>
       <c r="E94" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>98</v>
       </c>
@@ -2938,7 +2944,7 @@
         <v>0</v>
       </c>
       <c r="C95" s="2">
-        <v>-2.4756</v>
+        <v>-684.08385139137897</v>
       </c>
       <c r="D95" s="2">
         <v>0</v>
@@ -2947,97 +2953,97 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>99</v>
       </c>
       <c r="B96" s="2">
-        <v>-5.2775999999999996</v>
+        <v>-18.046573957987199</v>
       </c>
       <c r="C96" s="2">
-        <v>-5.2775999999999996</v>
+        <v>-957.75024004055604</v>
       </c>
       <c r="D96" s="2">
-        <v>-5.2775999999999996</v>
+        <v>-1819.74555434383</v>
       </c>
       <c r="E96" s="2">
-        <v>-5.2775999999999996</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1688.2461380468401</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>100</v>
       </c>
       <c r="B97" s="2">
-        <v>-3.6377999999999999</v>
+        <v>-49.991033591581399</v>
       </c>
       <c r="C97" s="2">
-        <v>-3.6377999999999999</v>
+        <v>-1000.32800325165</v>
       </c>
       <c r="D97" s="2">
-        <v>-3.6377999999999999</v>
+        <v>-1826.4487962068599</v>
       </c>
       <c r="E97" s="2">
-        <v>-3.6377999999999999</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1460.2529072059399</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>101</v>
       </c>
       <c r="B98" s="2">
-        <v>-8.6318000000000001</v>
+        <v>-5.67861865065984</v>
       </c>
       <c r="C98" s="2">
-        <v>-8.6318000000000001</v>
+        <v>-922.62713114530004</v>
       </c>
       <c r="D98" s="2">
-        <v>-8.6318000000000001</v>
+        <v>-1783.3428891651899</v>
       </c>
       <c r="E98" s="2">
-        <v>-8.6318000000000001</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1565.1169582084301</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B99" s="2">
-        <v>-3.4641999999999999</v>
+        <v>-65.107941620862206</v>
       </c>
       <c r="C99" s="2">
-        <v>-3.4641999999999999</v>
+        <v>-855.87399935141195</v>
       </c>
       <c r="D99" s="2">
-        <v>-3.4641999999999999</v>
+        <v>-1452.24045706727</v>
       </c>
       <c r="E99" s="2">
-        <v>-3.4641999999999999</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1736.19547301578</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B100" s="2">
-        <v>-4.6277999999999997</v>
+        <v>-42.730620602048702</v>
       </c>
       <c r="C100" s="2">
-        <v>-4.6277999999999997</v>
+        <v>-966.67307690033897</v>
       </c>
       <c r="D100" s="2">
-        <v>-4.6277999999999997</v>
+        <v>-1696.7337570080699</v>
       </c>
       <c r="E100" s="2">
-        <v>-4.6277999999999997</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1745.69180488558</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B101" s="2">
-        <v>-3.4098999999999999</v>
+        <v>-134.276163779575</v>
       </c>
       <c r="C101" s="2">
         <v>0</v>
@@ -3046,69 +3052,69 @@
         <v>0</v>
       </c>
       <c r="E101" s="2">
-        <v>-3.4098999999999999</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1644.65232964906</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>105</v>
       </c>
       <c r="B102" s="2">
-        <v>-11.3225</v>
+        <v>-19.324485699248999</v>
       </c>
       <c r="C102" s="2">
-        <v>-11.3225</v>
+        <v>-975.78359236455503</v>
       </c>
       <c r="D102" s="2">
-        <v>-11.3225</v>
+        <v>-1823.60324369821</v>
       </c>
       <c r="E102" s="2">
-        <v>-11.3225</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1682.1399209495701</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>106</v>
       </c>
       <c r="B103" s="2">
-        <v>-5.5641999999999996</v>
+        <v>-16.320855907915998</v>
       </c>
       <c r="C103" s="2">
-        <v>-5.5641999999999996</v>
+        <v>-933.07569780554797</v>
       </c>
       <c r="D103" s="2">
-        <v>-5.5641999999999996</v>
+        <v>-1817.7939674642801</v>
       </c>
       <c r="E103" s="2">
-        <v>-5.5641999999999996</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1591.6160379681801</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>107</v>
       </c>
       <c r="B104" s="2">
-        <v>-5.7210000000000001</v>
+        <v>-9.7265333598059005</v>
       </c>
       <c r="C104" s="2">
-        <v>-5.7210000000000001</v>
+        <v>-847.03358622765404</v>
       </c>
       <c r="D104" s="2">
-        <v>-5.7210000000000001</v>
+        <v>-1486.85996772109</v>
       </c>
       <c r="E104" s="2">
-        <v>-5.7210000000000001</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1689.4538706717599</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>108</v>
       </c>
       <c r="B105" s="2">
-        <v>-4.0849000000000002</v>
+        <v>-49.703588062706103</v>
       </c>
       <c r="C105" s="2">
-        <v>-4.0849000000000002</v>
+        <v>-934.44412342002101</v>
       </c>
       <c r="D105" s="2">
         <v>0</v>
@@ -3117,12 +3123,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>109</v>
       </c>
       <c r="B106" s="2">
-        <v>-3.2393999999999998</v>
+        <v>-87.075660277109705</v>
       </c>
       <c r="C106" s="2">
         <v>0</v>
@@ -3134,92 +3140,92 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B107" s="2">
-        <v>-3.7238000000000002</v>
+        <v>-32.051849812232298</v>
       </c>
       <c r="C107" s="2">
-        <v>-3.7238000000000002</v>
+        <v>-951.61985503788196</v>
       </c>
       <c r="D107" s="2">
         <v>0</v>
       </c>
       <c r="E107" s="2">
-        <v>-3.7238000000000002</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1675.8488984309299</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>111</v>
       </c>
       <c r="B108" s="2">
-        <v>-6.8265000000000002</v>
+        <v>-13.603435221264601</v>
       </c>
       <c r="C108" s="2">
-        <v>-6.8265000000000002</v>
+        <v>-633.29699508128704</v>
       </c>
       <c r="D108" s="2">
-        <v>-6.8265000000000002</v>
+        <v>-1514.62379341782</v>
       </c>
       <c r="E108" s="2">
-        <v>-6.8265000000000002</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1679.91950301612</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B109" s="2">
-        <v>-5.1441999999999997</v>
+        <v>-28.6789201214015</v>
       </c>
       <c r="C109" s="2">
-        <v>-5.1441999999999997</v>
+        <v>-973.52505274887505</v>
       </c>
       <c r="D109" s="2">
-        <v>-5.1441999999999997</v>
+        <v>-1799.0105828788201</v>
       </c>
       <c r="E109" s="2">
-        <v>-5.1441999999999997</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1647.07544419533</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>113</v>
       </c>
       <c r="B110" s="2">
-        <v>-7.1901999999999999</v>
+        <v>-40.327705666284402</v>
       </c>
       <c r="C110" s="2">
-        <v>-7.1901999999999999</v>
+        <v>-912.36712424352004</v>
       </c>
       <c r="D110" s="2">
-        <v>-7.1901999999999999</v>
+        <v>-1810.5694964132199</v>
       </c>
       <c r="E110" s="2">
-        <v>-7.1901999999999999</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1686.67786466866</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>114</v>
       </c>
       <c r="B111" s="2">
-        <v>-3.9003000000000001</v>
+        <v>-43.208563066971003</v>
       </c>
       <c r="C111" s="2">
-        <v>-3.9003000000000001</v>
+        <v>-834.70597531280396</v>
       </c>
       <c r="D111" s="2">
-        <v>-3.9003000000000001</v>
+        <v>-1829.3085153674899</v>
       </c>
       <c r="E111" s="2">
-        <v>-3.9003000000000001</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1661.7891397130199</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>115</v>
       </c>
@@ -3227,50 +3233,50 @@
         <v>0</v>
       </c>
       <c r="C112" s="2">
-        <v>-2.6648000000000001</v>
+        <v>-966.56143578401498</v>
       </c>
       <c r="D112" s="2">
-        <v>-2.6648000000000001</v>
+        <v>-1627.3350709699</v>
       </c>
       <c r="E112" s="2">
-        <v>-2.6648000000000001</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1711.09099554404</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>116</v>
       </c>
       <c r="B113" s="2">
-        <v>-5.0559000000000003</v>
+        <v>-100.328603128634</v>
       </c>
       <c r="C113" s="2">
-        <v>-5.0559000000000003</v>
+        <v>-942.04000076520197</v>
       </c>
       <c r="D113" s="2">
-        <v>-5.0559000000000003</v>
+        <v>-1824.33371303987</v>
       </c>
       <c r="E113" s="2">
-        <v>-5.0559000000000003</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1698.18482044192</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>117</v>
       </c>
       <c r="B114" s="2">
-        <v>-9.468</v>
+        <v>-38.886676022166597</v>
       </c>
       <c r="C114" s="2">
-        <v>-9.468</v>
+        <v>-972.47412862917304</v>
       </c>
       <c r="D114" s="2">
-        <v>-9.468</v>
+        <v>-1809.1156498979799</v>
       </c>
       <c r="E114" s="2">
-        <v>-9.468</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1667.10127855051</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>118</v>
       </c>
@@ -3281,30 +3287,30 @@
         <v>0</v>
       </c>
       <c r="D115" s="2">
-        <v>-3.4872000000000001</v>
+        <v>-1524.61242604923</v>
       </c>
       <c r="E115" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>119</v>
       </c>
       <c r="B116" s="2">
-        <v>-7.4218999999999999</v>
+        <v>-76.175776558368597</v>
       </c>
       <c r="C116" s="2">
-        <v>-7.4218999999999999</v>
+        <v>-965.89781823338001</v>
       </c>
       <c r="D116" s="2">
-        <v>-7.4218999999999999</v>
+        <v>-1813.1252691785101</v>
       </c>
       <c r="E116" s="2">
-        <v>-7.4218999999999999</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1695.8891414898701</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>120</v>
       </c>
@@ -3318,61 +3324,61 @@
         <v>0</v>
       </c>
       <c r="E117" s="2">
-        <v>-2.2921999999999998</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1673.34159882426</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>121</v>
       </c>
       <c r="B118" s="2">
-        <v>-5.1615000000000002</v>
+        <v>11.2788396125465</v>
       </c>
       <c r="C118" s="2">
-        <v>-5.1615000000000002</v>
+        <v>-958.80691057972103</v>
       </c>
       <c r="D118" s="2">
-        <v>-5.1615000000000002</v>
+        <v>-1762.71323671602</v>
       </c>
       <c r="E118" s="2">
-        <v>-5.1615000000000002</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1489.68957335096</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>122</v>
       </c>
       <c r="B119" s="2">
-        <v>-4.0205000000000002</v>
+        <v>-6.3173952342382202</v>
       </c>
       <c r="C119" s="2">
-        <v>-4.0205000000000002</v>
+        <v>-970.92789436915496</v>
       </c>
       <c r="D119" s="2">
-        <v>-4.0205000000000002</v>
+        <v>-1791.7436643946501</v>
       </c>
       <c r="E119" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>123</v>
       </c>
       <c r="B120" s="2">
-        <v>-5.4309000000000003</v>
+        <v>21.8387172667904</v>
       </c>
       <c r="C120" s="2">
-        <v>-5.4309000000000003</v>
+        <v>-674.67880940033501</v>
       </c>
       <c r="D120" s="2">
-        <v>-5.4309000000000003</v>
+        <v>-1534.63527891637</v>
       </c>
       <c r="E120" s="2">
-        <v>-5.4309000000000003</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1660.9363064689901</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>124</v>
       </c>
@@ -3386,27 +3392,27 @@
         <v>0</v>
       </c>
       <c r="E121" s="2">
-        <v>-3.1686999999999999</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1505.23868706604</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>125</v>
       </c>
       <c r="B122" s="2">
-        <v>-7.8776000000000002</v>
+        <v>-29.899161864475801</v>
       </c>
       <c r="C122" s="2">
-        <v>-7.8776000000000002</v>
+        <v>-934.05584863878403</v>
       </c>
       <c r="D122" s="2">
-        <v>-7.8776000000000002</v>
+        <v>-1827.6991045247401</v>
       </c>
       <c r="E122" s="2">
-        <v>-7.8776000000000002</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1656.1850741058299</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>126</v>
       </c>
@@ -3417,132 +3423,132 @@
         <v>0</v>
       </c>
       <c r="D123" s="2">
-        <v>-2.2860999999999998</v>
+        <v>-1743.11960872123</v>
       </c>
       <c r="E123" s="2">
-        <v>-2.2860999999999998</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1491.7330119257099</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>127</v>
       </c>
       <c r="B124" s="2">
-        <v>-4.4118000000000004</v>
+        <v>-82.315317801860203</v>
       </c>
       <c r="C124" s="2">
-        <v>-4.4118000000000004</v>
+        <v>-899.301719801216</v>
       </c>
       <c r="D124" s="2">
-        <v>-4.4118000000000004</v>
+        <v>-1814.26076233617</v>
       </c>
       <c r="E124" s="2">
-        <v>-4.4118000000000004</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1472.93396121654</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>128</v>
       </c>
       <c r="B125" s="2">
-        <v>-2.7917999999999998</v>
+        <v>-12.2093684915806</v>
       </c>
       <c r="C125" s="2">
         <v>0</v>
       </c>
       <c r="D125" s="2">
-        <v>-2.7917999999999998</v>
+        <v>-1802.0586931781399</v>
       </c>
       <c r="E125" s="2">
-        <v>-2.7917999999999998</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1620.5531137944399</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>129</v>
       </c>
       <c r="B126" s="2">
-        <v>-3.6560999999999999</v>
+        <v>-38.892926110388103</v>
       </c>
       <c r="C126" s="2">
-        <v>-3.6560999999999999</v>
+        <v>-941.61517660100799</v>
       </c>
       <c r="D126" s="2">
         <v>0</v>
       </c>
       <c r="E126" s="2">
-        <v>-3.6560999999999999</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1681.5669222720501</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>130</v>
       </c>
       <c r="B127" s="2">
-        <v>-4.8</v>
+        <v>5.9687820043876902</v>
       </c>
       <c r="C127" s="2">
-        <v>-4.8</v>
+        <v>-978.14910858342796</v>
       </c>
       <c r="D127" s="2">
-        <v>-4.8</v>
+        <v>-1805.8884136762599</v>
       </c>
       <c r="E127" s="2">
-        <v>-4.8</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1679.0250178828801</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>131</v>
       </c>
       <c r="B128" s="2">
-        <v>-7.0247999999999999</v>
+        <v>25.427988677237401</v>
       </c>
       <c r="C128" s="2">
-        <v>-7.0247999999999999</v>
+        <v>-797.86523754099505</v>
       </c>
       <c r="D128" s="2">
-        <v>-7.0247999999999999</v>
+        <v>-1559.0122027678501</v>
       </c>
       <c r="E128" s="2">
-        <v>-7.0247999999999999</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1692.68861986251</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>132</v>
       </c>
       <c r="B129" s="2">
-        <v>-3.8614999999999999</v>
+        <v>14.1115002244766</v>
       </c>
       <c r="C129" s="2">
-        <v>-3.8614999999999999</v>
+        <v>-904.69621961359496</v>
       </c>
       <c r="D129" s="2">
-        <v>-3.8614999999999999</v>
+        <v>-1712.3754410664801</v>
       </c>
       <c r="E129" s="2">
-        <v>-3.8614999999999999</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1558.5268307041299</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>133</v>
       </c>
       <c r="B130" s="2">
-        <v>-4.5688000000000004</v>
+        <v>13.0343576823647</v>
       </c>
       <c r="C130" s="2">
-        <v>-4.5688000000000004</v>
+        <v>-906.00388000354997</v>
       </c>
       <c r="D130" s="2">
-        <v>-4.5688000000000004</v>
+        <v>-1671.71002585474</v>
       </c>
       <c r="E130" s="2">
-        <v>-4.5688000000000004</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1622.0367014866799</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>134</v>
       </c>
@@ -3550,135 +3556,135 @@
         <v>0</v>
       </c>
       <c r="C131" s="2">
-        <v>-4.2375999999999996</v>
+        <v>-927.59123676993499</v>
       </c>
       <c r="D131" s="2">
-        <v>-4.2375999999999996</v>
+        <v>-1605.0139156066</v>
       </c>
       <c r="E131" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>135</v>
       </c>
       <c r="B132" s="2">
-        <v>-5.2991000000000001</v>
+        <v>-70.728715525319203</v>
       </c>
       <c r="C132" s="2">
-        <v>-5.2991000000000001</v>
+        <v>-956.89453385007096</v>
       </c>
       <c r="D132" s="2">
-        <v>-5.2991000000000001</v>
+        <v>-1813.29686890738</v>
       </c>
       <c r="E132" s="2">
-        <v>-5.2991000000000001</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1712.62916237168</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>136</v>
       </c>
       <c r="B133" s="2">
-        <v>-4.6656000000000004</v>
+        <v>-57.245244300315903</v>
       </c>
       <c r="C133" s="2">
-        <v>-4.6656000000000004</v>
+        <v>-958.12944655637205</v>
       </c>
       <c r="D133" s="2">
         <v>0</v>
       </c>
       <c r="E133" s="2">
-        <v>-4.6656000000000004</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1656.48351612174</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>137</v>
       </c>
       <c r="B134" s="2">
-        <v>-9.2431999999999999</v>
+        <v>-89.684432225447395</v>
       </c>
       <c r="C134" s="2">
-        <v>-9.2431999999999999</v>
+        <v>-431.80147497022301</v>
       </c>
       <c r="D134" s="2">
-        <v>-9.2431999999999999</v>
+        <v>-1176.0148746050299</v>
       </c>
       <c r="E134" s="2">
-        <v>-9.2431999999999999</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1650.49100317283</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>138</v>
       </c>
       <c r="B135" s="2">
-        <v>-4.7191999999999998</v>
+        <v>12.6427872045681</v>
       </c>
       <c r="C135" s="2">
-        <v>-4.7191999999999998</v>
+        <v>-825.681611850683</v>
       </c>
       <c r="D135" s="2">
-        <v>-4.7191999999999998</v>
+        <v>-1660.0409037572299</v>
       </c>
       <c r="E135" s="2">
-        <v>-4.7191999999999998</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1666.5032200416999</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>139</v>
       </c>
       <c r="B136" s="2">
-        <v>-4.5830000000000002</v>
+        <v>-4.0212554439750603</v>
       </c>
       <c r="C136" s="2">
-        <v>-4.5830000000000002</v>
+        <v>-959.075208999506</v>
       </c>
       <c r="D136" s="2">
-        <v>-4.5830000000000002</v>
+        <v>-1730.81686365719</v>
       </c>
       <c r="E136" s="2">
-        <v>-4.5830000000000002</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1667.3402915793499</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>140</v>
       </c>
       <c r="B137" s="2">
-        <v>-7.4046000000000003</v>
+        <v>-35.806819192300601</v>
       </c>
       <c r="C137" s="2">
-        <v>-7.4046000000000003</v>
+        <v>-965.55438247825998</v>
       </c>
       <c r="D137" s="2">
-        <v>-7.4046000000000003</v>
+        <v>-1823.8905310154801</v>
       </c>
       <c r="E137" s="2">
-        <v>-7.4046000000000003</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1658.6533344347899</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>141</v>
       </c>
       <c r="B138" s="2">
-        <v>-5.6890999999999998</v>
+        <v>21.178712516945598</v>
       </c>
       <c r="C138" s="2">
-        <v>-5.6890999999999998</v>
+        <v>-840.759617795503</v>
       </c>
       <c r="D138" s="2">
-        <v>-5.6890999999999998</v>
+        <v>-1741.1690494337399</v>
       </c>
       <c r="E138" s="2">
-        <v>-5.6890999999999998</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1692.69370187923</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>142</v>
       </c>
@@ -3695,7 +3701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>143</v>
       </c>
@@ -3703,7 +3709,7 @@
         <v>0</v>
       </c>
       <c r="C140" s="2">
-        <v>-2.6856</v>
+        <v>-955.15811269772701</v>
       </c>
       <c r="D140" s="2">
         <v>0</v>
@@ -3712,109 +3718,109 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>144</v>
       </c>
       <c r="B141" s="2">
-        <v>-5.7477</v>
+        <v>-37.587714098439399</v>
       </c>
       <c r="C141" s="2">
-        <v>-5.7477</v>
+        <v>-966.64935169233104</v>
       </c>
       <c r="D141" s="2">
-        <v>-5.7477</v>
+        <v>-1787.6442831024599</v>
       </c>
       <c r="E141" s="2">
-        <v>-5.7477</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1524.81738448086</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>145</v>
       </c>
       <c r="B142" s="2">
-        <v>-4.2439999999999998</v>
+        <v>27.7457297478139</v>
       </c>
       <c r="C142" s="2">
-        <v>-4.2439999999999998</v>
+        <v>-917.15583846437903</v>
       </c>
       <c r="D142" s="2">
-        <v>-4.2439999999999998</v>
+        <v>-1721.38765690163</v>
       </c>
       <c r="E142" s="2">
-        <v>-4.2439999999999998</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1523.77487414857</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>146</v>
       </c>
       <c r="B143" s="2">
-        <v>-5.3548</v>
+        <v>-62.454102020546799</v>
       </c>
       <c r="C143" s="2">
-        <v>-5.3548</v>
+        <v>-959.71915277689595</v>
       </c>
       <c r="D143" s="2">
-        <v>-5.3548</v>
+        <v>-1774.79579468309</v>
       </c>
       <c r="E143" s="2">
-        <v>-5.3548</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1499.7259070489899</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>147</v>
       </c>
       <c r="B144" s="2">
-        <v>-5.7698999999999998</v>
+        <v>-62.690153890653903</v>
       </c>
       <c r="C144" s="2">
-        <v>-5.7698999999999998</v>
+        <v>-958.18963276020997</v>
       </c>
       <c r="D144" s="2">
-        <v>-5.7698999999999998</v>
+        <v>-1547.8295971007899</v>
       </c>
       <c r="E144" s="2">
-        <v>-5.7698999999999998</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1802.1445668020699</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>148</v>
       </c>
       <c r="B145" s="2">
-        <v>-6.2774999999999999</v>
+        <v>-105.046337300698</v>
       </c>
       <c r="C145" s="2">
-        <v>-6.2774999999999999</v>
+        <v>-986.79996534697898</v>
       </c>
       <c r="D145" s="2">
-        <v>-6.2774999999999999</v>
+        <v>-1808.13570293366</v>
       </c>
       <c r="E145" s="2">
-        <v>-6.2774999999999999</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1671.8221651200899</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>149</v>
       </c>
       <c r="B146" s="2">
-        <v>-4.9626999999999999</v>
+        <v>-15.125301736907399</v>
       </c>
       <c r="C146" s="2">
-        <v>-4.9626999999999999</v>
+        <v>-944.25779668419204</v>
       </c>
       <c r="D146" s="2">
-        <v>-4.9626999999999999</v>
+        <v>-1780.87989918225</v>
       </c>
       <c r="E146" s="2">
-        <v>-4.9626999999999999</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1605.44663348362</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>150</v>
       </c>
@@ -3831,75 +3837,75 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
         <v>151</v>
       </c>
       <c r="B148" s="2">
-        <v>-6.3112000000000004</v>
+        <v>-3.5109346735850502</v>
       </c>
       <c r="C148" s="2">
-        <v>-6.3112000000000004</v>
+        <v>-961.62574114618701</v>
       </c>
       <c r="D148" s="2">
-        <v>-6.3112000000000004</v>
+        <v>-1808.0308463778399</v>
       </c>
       <c r="E148" s="2">
-        <v>-6.3112000000000004</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1755.7537110171199</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
         <v>152</v>
       </c>
       <c r="B149" s="2">
-        <v>-7.5559000000000003</v>
+        <v>-21.302113524714802</v>
       </c>
       <c r="C149" s="2">
-        <v>-7.5559000000000003</v>
+        <v>-958.47582378305196</v>
       </c>
       <c r="D149" s="2">
-        <v>-7.5559000000000003</v>
+        <v>-1725.72006785843</v>
       </c>
       <c r="E149" s="2">
-        <v>-7.5559000000000003</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1814.8567127799499</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
         <v>153</v>
       </c>
       <c r="B150" s="2">
-        <v>-5.1776999999999997</v>
+        <v>8.2456498610865996</v>
       </c>
       <c r="C150" s="2">
-        <v>-5.1776999999999997</v>
+        <v>-896.57134651645595</v>
       </c>
       <c r="D150" s="2">
-        <v>-5.1776999999999997</v>
+        <v>-1733.2763335424499</v>
       </c>
       <c r="E150" s="2">
-        <v>-5.1776999999999997</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1435.4986902370399</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
         <v>154</v>
       </c>
       <c r="B151" s="2">
-        <v>-8.0014000000000003</v>
+        <v>34.949409660745602</v>
       </c>
       <c r="C151" s="2">
-        <v>-8.0014000000000003</v>
+        <v>-965.79767576518702</v>
       </c>
       <c r="D151" s="2">
-        <v>-8.0014000000000003</v>
+        <v>-1786.57129132009</v>
       </c>
       <c r="E151" s="2">
-        <v>-8.0014000000000003</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1483.8235046985601</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
         <v>155</v>
       </c>
@@ -3913,10 +3919,10 @@
         <v>0</v>
       </c>
       <c r="E152" s="2">
-        <v>-3.0998999999999999</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1548.31671941595</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
         <v>156</v>
       </c>
@@ -3924,10 +3930,10 @@
         <v>0</v>
       </c>
       <c r="C153" s="2">
-        <v>-3.1905000000000001</v>
+        <v>-626.43460377891995</v>
       </c>
       <c r="D153" s="2">
-        <v>-3.1905000000000001</v>
+        <v>-1666.42942200926</v>
       </c>
       <c r="E153" s="2">
         <v>0</v>
@@ -3950,9 +3956,9 @@
       <selection sqref="A1:E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>0</v>
       </c>
@@ -3969,7 +3975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3986,7 +3992,7 @@
         <v>1.9599999999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>0</v>
       </c>
@@ -4003,7 +4009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0</v>
       </c>
@@ -4020,7 +4026,7 @@
         <v>6.6E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>0.12889999999999999</v>
       </c>
@@ -4037,7 +4043,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>0.97160000000000002</v>
       </c>
@@ -4054,7 +4060,7 @@
         <v>1.1999999999999999E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>0</v>
       </c>
@@ -4071,7 +4077,7 @@
         <v>8.2699999999999996E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3.3000000000000002E-2</v>
       </c>
@@ -4088,7 +4094,7 @@
         <v>0.95269999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1E-4</v>
       </c>
@@ -4105,7 +4111,7 @@
         <v>0.123</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1E-4</v>
       </c>
@@ -4122,7 +4128,7 @@
         <v>0.97570000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1.1000000000000001E-3</v>
       </c>
@@ -4139,7 +4145,7 @@
         <v>0.87180000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>0.89939999999999998</v>
       </c>
@@ -4156,7 +4162,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>0</v>
       </c>
@@ -4173,7 +4179,7 @@
         <v>8.2900000000000001E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>0</v>
       </c>
@@ -4190,7 +4196,7 @@
         <v>0.53069999999999995</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>0.87450000000000006</v>
       </c>
@@ -4207,7 +4213,7 @@
         <v>2.1100000000000001E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>0</v>
       </c>
@@ -4224,7 +4230,7 @@
         <v>0.81510000000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1E-4</v>
       </c>
@@ -4241,7 +4247,7 @@
         <v>0.123</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>0</v>
       </c>
@@ -4258,7 +4264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>0</v>
       </c>
@@ -4275,7 +4281,7 @@
         <v>6.6E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>0.98629999999999995</v>
       </c>
@@ -4303,7 +4309,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add new disease/treatment information to 4.2.
Updated disease information provides for more variation in VOI
computations.
</commit_message>
<xml_diff>
--- a/solutions/problem2/problem-2-solution-voi.xlsx
+++ b/solutions/problem2/problem-2-solution-voi.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin-slater\gh\ppaml-cp4\solutions\problem2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OSUAcademics\PPAML\CP4_works\Problem2_MedicalDiagnosis\updated_for_corrected_voi_March_9_2015\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="96" windowWidth="16272" windowHeight="7236"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="16275" windowHeight="7230"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1338,15 +1338,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E153"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" style="2" customWidth="1"/>
-    <col min="2" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="1" width="10.85546875" style="2" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1357,7 +1359,7 @@
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -1372,41 +1374,41 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2">
-        <v>-110.31516426844399</v>
+        <v>159.00022241545901</v>
       </c>
       <c r="C3" s="2">
         <v>0</v>
       </c>
       <c r="D3" s="2">
-        <v>-1848.1753687029</v>
+        <v>-958.63932717511602</v>
       </c>
       <c r="E3" s="2">
-        <v>-1665.35668249536</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7.37704335082572</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="2">
-        <v>-112.994959703234</v>
+        <v>133.88215416931101</v>
       </c>
       <c r="C4" s="2">
-        <v>-903.79563969236494</v>
+        <v>-725.88975798224999</v>
       </c>
       <c r="D4" s="2">
-        <v>-1324.4890770602799</v>
+        <v>-422.15381109691901</v>
       </c>
       <c r="E4" s="2">
-        <v>-1789.41519615985</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-133.07947090436099</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1414,50 +1416,50 @@
         <v>0</v>
       </c>
       <c r="C5" s="2">
-        <v>-958.55303776867402</v>
+        <v>-789.70149565278098</v>
       </c>
       <c r="D5" s="2">
-        <v>-1827.11824411875</v>
+        <v>-943.932081692157</v>
       </c>
       <c r="E5" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="2">
-        <v>-26.230830025593601</v>
+        <v>243.37488758829599</v>
       </c>
       <c r="C6" s="2">
-        <v>-934.81557855563199</v>
+        <v>-763.32604479285999</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
       </c>
       <c r="E6" s="2">
-        <v>-1629.0417332685799</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-49.099207900518401</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="2">
-        <v>-18.4370378088088</v>
+        <v>243.05896873627401</v>
       </c>
       <c r="C7" s="2">
-        <v>-958.49144594745405</v>
+        <v>-788.151507518838</v>
       </c>
       <c r="D7" s="2">
-        <v>-1821.39340573923</v>
+        <v>-941.78652687962904</v>
       </c>
       <c r="E7" s="2">
-        <v>-1712.04276010334</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-17.269966938867899</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -1465,7 +1467,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="2">
-        <v>-870.01396242122701</v>
+        <v>-715.77033931717403</v>
       </c>
       <c r="D8" s="2">
         <v>0</v>
@@ -1474,7 +1476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -1485,98 +1487,98 @@
         <v>0</v>
       </c>
       <c r="D9" s="2">
-        <v>-1588.48969505642</v>
+        <v>-964.25099799818202</v>
       </c>
       <c r="E9" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="2">
-        <v>-162.57388545734699</v>
+        <v>-11.8707071978865</v>
       </c>
       <c r="C10" s="2">
-        <v>-954.98323603708297</v>
+        <v>-880.81832999171604</v>
       </c>
       <c r="D10" s="2">
-        <v>-1801.83980452623</v>
+        <v>-1052.2178752493101</v>
       </c>
       <c r="E10" s="2">
-        <v>-1694.82386934489</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-161.279640101963</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="2">
-        <v>19.581024875347101</v>
+        <v>-405.972779721226</v>
       </c>
       <c r="C11" s="2">
-        <v>-782.94856629690003</v>
+        <v>-1305.99125711498</v>
       </c>
       <c r="D11" s="2">
-        <v>-1634.1332619858999</v>
+        <v>-1454.3249567677101</v>
       </c>
       <c r="E11" s="2">
-        <v>-1680.1148162305501</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-698.66779898921595</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="2">
-        <v>13.634870629455101</v>
+        <v>260.50808291962198</v>
       </c>
       <c r="C12" s="2">
-        <v>-896.98189281574298</v>
+        <v>-741.59030351577996</v>
       </c>
       <c r="D12" s="2">
-        <v>-1791.40428846226</v>
+        <v>-914.71229751082205</v>
       </c>
       <c r="E12" s="2">
-        <v>-1683.18638635506</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-5.60967884118645</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="2">
-        <v>-39.559889176117203</v>
+        <v>225.889123503131</v>
       </c>
       <c r="C13" s="2">
-        <v>-723.88291732329196</v>
+        <v>-567.57922627318897</v>
       </c>
       <c r="D13" s="2">
-        <v>-1534.5464094378201</v>
+        <v>-689.37407768284197</v>
       </c>
       <c r="E13" s="2">
-        <v>-1634.7913646135601</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>22.401778460561701</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="2">
-        <v>-67.375854871904707</v>
+        <v>192.19027774992401</v>
       </c>
       <c r="C14" s="2">
-        <v>-928.36788629660998</v>
+        <v>-758.63710772514798</v>
       </c>
       <c r="D14" s="2">
-        <v>-1831.3429981854299</v>
+        <v>-946.68085007584705</v>
       </c>
       <c r="E14" s="2">
-        <v>-1698.0873769398099</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-11.859039717498201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
@@ -1584,50 +1586,50 @@
         <v>0</v>
       </c>
       <c r="C15" s="2">
-        <v>-589.26960549022499</v>
+        <v>-482.43531542456202</v>
       </c>
       <c r="D15" s="2">
-        <v>-1786.1173105811399</v>
+        <v>-907.64759904537902</v>
       </c>
       <c r="E15" s="2">
-        <v>-1633.03607839652</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <v>14.6943053925424</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B16" s="2">
-        <v>-3.01786206799602</v>
+        <v>263.30393233660402</v>
       </c>
       <c r="C16" s="2">
-        <v>-680.32035426247705</v>
+        <v>-513.103437027327</v>
       </c>
       <c r="D16" s="2">
-        <v>-1565.09059022613</v>
+        <v>-689.86455829693705</v>
       </c>
       <c r="E16" s="2">
-        <v>-1677.7524909891599</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-3.50955194544576</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="2">
-        <v>-77.534444352913695</v>
+        <v>180.509609714205</v>
       </c>
       <c r="C17" s="2">
-        <v>-961.08503079324498</v>
+        <v>-802.05312680883196</v>
       </c>
       <c r="D17" s="2">
-        <v>-1775.2344439093499</v>
+        <v>-917.565685272417</v>
       </c>
       <c r="E17" s="2">
-        <v>-1627.1184861418601</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-28.332045258955699</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
@@ -1638,13 +1640,13 @@
         <v>0</v>
       </c>
       <c r="D18" s="2">
-        <v>-1806.58077662084</v>
+        <v>-923.57519946584705</v>
       </c>
       <c r="E18" s="2">
-        <v>-1712.46838766105</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-31.596193137622699</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
@@ -1658,44 +1660,44 @@
         <v>0</v>
       </c>
       <c r="E19" s="2">
-        <v>-1707.9824767733601</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-26.017437557553201</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B20" s="2">
-        <v>-54.938361870946899</v>
+        <v>209.20245347892001</v>
       </c>
       <c r="C20" s="2">
-        <v>-859.93028094261297</v>
+        <v>-680.820074569638</v>
       </c>
       <c r="D20" s="2">
         <v>0</v>
       </c>
       <c r="E20" s="2">
-        <v>-1671.9188469196999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1.9119241320320299</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B21" s="2">
-        <v>-38.131097966687499</v>
+        <v>234.68019004416399</v>
       </c>
       <c r="C21" s="2">
-        <v>-946.42296303884996</v>
+        <v>-780.801263709561</v>
       </c>
       <c r="D21" s="2">
-        <v>-1790.8550584597299</v>
+        <v>-896.31081068216895</v>
       </c>
       <c r="E21" s="2">
-        <v>-1676.6280650315</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+        <v>4.4234150259348999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>25</v>
       </c>
@@ -1703,16 +1705,16 @@
         <v>0</v>
       </c>
       <c r="C22" s="2">
-        <v>-948.60657604286803</v>
+        <v>-768.03692722991195</v>
       </c>
       <c r="D22" s="2">
-        <v>-1737.55493226261</v>
+        <v>-853.22150612983501</v>
       </c>
       <c r="E22" s="2">
-        <v>-1672.8874354223501</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1.82004981050341</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
@@ -1729,29 +1731,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="2">
-        <v>-57.294920939978098</v>
+        <v>198.12789239946699</v>
       </c>
       <c r="C24" s="2">
-        <v>-952.41103531937995</v>
+        <v>-786.21692899535299</v>
       </c>
       <c r="D24" s="2">
-        <v>-1752.8420326078301</v>
+        <v>-916.57661774013695</v>
       </c>
       <c r="E24" s="2">
-        <v>-1533.3587450799901</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-18.111016957727799</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B25" s="2">
-        <v>31.1798421792375</v>
+        <v>283.56752164557599</v>
       </c>
       <c r="C25" s="2">
         <v>0</v>
@@ -1763,63 +1765,63 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B26" s="2">
-        <v>13.857312611223101</v>
+        <v>241.08800161416701</v>
       </c>
       <c r="C26" s="2">
-        <v>-690.97070768811795</v>
+        <v>-580.99153850003597</v>
       </c>
       <c r="D26" s="2">
-        <v>-1806.37335417194</v>
+        <v>-923.18922786736698</v>
       </c>
       <c r="E26" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B27" s="2">
-        <v>-97.653596985239901</v>
+        <v>-75.216435050254404</v>
       </c>
       <c r="C27" s="2">
-        <v>-973.78058160717501</v>
+        <v>-1020.36522552617</v>
       </c>
       <c r="D27" s="2">
-        <v>-1487.3962418485301</v>
+        <v>-1194.4477512778999</v>
       </c>
       <c r="E27" s="2">
-        <v>-1577.68420325178</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-271.599548392136</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B28" s="2">
-        <v>20.7833485731264</v>
+        <v>288.43722210976102</v>
       </c>
       <c r="C28" s="2">
-        <v>-793.515847411256</v>
+        <v>-625.14808146424502</v>
       </c>
       <c r="D28" s="2">
-        <v>-1508.1976557657099</v>
+        <v>-825.43539412445102</v>
       </c>
       <c r="E28" s="2">
-        <v>-1706.96163877709</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-5.4563845759564602</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B29" s="2">
-        <v>-46.787656013303398</v>
+        <v>203.583939506983</v>
       </c>
       <c r="C29" s="2">
         <v>0</v>
@@ -1831,58 +1833,58 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B30" s="2">
-        <v>-40.574524052293</v>
+        <v>218.57645917006701</v>
       </c>
       <c r="C30" s="2">
-        <v>-951.18501444453</v>
+        <v>-791.19793865591805</v>
       </c>
       <c r="D30" s="2">
-        <v>-1793.3945657469301</v>
+        <v>-927.64628387017694</v>
       </c>
       <c r="E30" s="2">
-        <v>-1732.4238255355999</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-60.673076040487601</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B31" s="2">
-        <v>-33.069148170210802</v>
+        <v>216.132823067392</v>
       </c>
       <c r="C31" s="2">
-        <v>-905.69126349663998</v>
+        <v>-751.13804195093996</v>
       </c>
       <c r="D31" s="2">
-        <v>-1786.4779429965099</v>
+        <v>-927.913990030175</v>
       </c>
       <c r="E31" s="2">
-        <v>-1618.6541443102001</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-43.289070574351399</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B32" s="2">
-        <v>0.79457328950628403</v>
+        <v>263.93228568541502</v>
       </c>
       <c r="C32" s="2">
-        <v>-954.05893657795696</v>
+        <v>-787.157578935586</v>
       </c>
       <c r="D32" s="2">
-        <v>-1814.8559782464399</v>
+        <v>-935.01792158345995</v>
       </c>
       <c r="E32" s="2">
-        <v>-1703.52355520624</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-18.740006603106099</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>36</v>
       </c>
@@ -1896,256 +1898,256 @@
         <v>0</v>
       </c>
       <c r="E33" s="2">
-        <v>-1685.2420552266899</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-28.722902408957999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B34" s="2">
-        <v>-44.314399411917201</v>
+        <v>147.97876715206999</v>
       </c>
       <c r="C34" s="2">
-        <v>-936.98815637377095</v>
+        <v>-802.58117607766803</v>
       </c>
       <c r="D34" s="2">
-        <v>-1821.1839162354499</v>
+        <v>-945.88929151145305</v>
       </c>
       <c r="E34" s="2">
-        <v>-1583.5085370250599</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+        <v>6.03166931926887</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B35" s="2">
-        <v>-50.169852465122403</v>
+        <v>198.90814201035701</v>
       </c>
       <c r="C35" s="2">
-        <v>-943.08124513084397</v>
+        <v>-780.07864937365696</v>
       </c>
       <c r="D35" s="2">
-        <v>-1824.38788012693</v>
+        <v>-949.49901431476599</v>
       </c>
       <c r="E35" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B36" s="2">
-        <v>-69.113180804199104</v>
+        <v>192.23217525081901</v>
       </c>
       <c r="C36" s="2">
-        <v>-968.50924135461003</v>
+        <v>-795.05027910324702</v>
       </c>
       <c r="D36" s="2">
-        <v>-1760.3025662600801</v>
+        <v>-893.414956459775</v>
       </c>
       <c r="E36" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B37" s="2">
-        <v>-33.376253118115201</v>
+        <v>229.68515078063001</v>
       </c>
       <c r="C37" s="2">
         <v>0</v>
       </c>
       <c r="D37" s="2">
-        <v>-1768.2301189065099</v>
+        <v>-893.11502099501695</v>
       </c>
       <c r="E37" s="2">
-        <v>-1674.8046293111299</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-19.856513317739299</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B38" s="2">
-        <v>-17.093136446910201</v>
+        <v>255.16231092067301</v>
       </c>
       <c r="C38" s="2">
-        <v>-941.30019204917198</v>
+        <v>-769.01951739909498</v>
       </c>
       <c r="D38" s="2">
-        <v>-1756.09920918021</v>
+        <v>-864.17125818467105</v>
       </c>
       <c r="E38" s="2">
-        <v>-1675.1687736687099</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-2.6672141227936699</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B39" s="2">
-        <v>31.023390190440999</v>
+        <v>261.76078844475597</v>
       </c>
       <c r="C39" s="2">
-        <v>-954.50917490959796</v>
+        <v>-785.67982456530797</v>
       </c>
       <c r="D39" s="2">
-        <v>-1737.21089482447</v>
+        <v>-915.89375189944496</v>
       </c>
       <c r="E39" s="2">
-        <v>-1661.6909357494901</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-1.18682754529573</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B40" s="2">
-        <v>-0.71975320167780399</v>
+        <v>265.60209661933902</v>
       </c>
       <c r="C40" s="2">
         <v>0</v>
       </c>
       <c r="D40" s="2">
-        <v>-1713.53982897264</v>
+        <v>-831.481989277926</v>
       </c>
       <c r="E40" s="2">
-        <v>-1677.49423205978</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-3.7185426739856702</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B41" s="2">
-        <v>4.9347099462102104</v>
+        <v>271.44961551946898</v>
       </c>
       <c r="C41" s="2">
-        <v>-589.61777350605598</v>
+        <v>-451.59954367476502</v>
       </c>
       <c r="D41" s="2">
-        <v>-1378.8848079505501</v>
+        <v>-545.60599444029594</v>
       </c>
       <c r="E41" s="2">
-        <v>-1708.15259390039</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-24.0092382190774</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B42" s="2">
-        <v>12.3457771781601</v>
+        <v>279.75927643328299</v>
       </c>
       <c r="C42" s="2">
-        <v>-964.48529324014203</v>
+        <v>-795.68941644234496</v>
       </c>
       <c r="D42" s="2">
-        <v>-1757.0664679338399</v>
+        <v>-871.88759717399296</v>
       </c>
       <c r="E42" s="2">
-        <v>-1665.97654643838</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+        <v>10.082542314463501</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B43" s="2">
-        <v>-33.322588440724303</v>
+        <v>199.04046206166601</v>
       </c>
       <c r="C43" s="2">
-        <v>-915.52592885690399</v>
+        <v>-759.46356007251495</v>
       </c>
       <c r="D43" s="2">
-        <v>-1724.56574652932</v>
+        <v>-935.25478686683698</v>
       </c>
       <c r="E43" s="2">
-        <v>-1566.82486529167</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-23.093456353742798</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>47</v>
       </c>
       <c r="B44" s="2">
-        <v>-46.748300822020198</v>
+        <v>175.05284715863601</v>
       </c>
       <c r="C44" s="2">
-        <v>-833.33859393265595</v>
+        <v>-707.17875643029697</v>
       </c>
       <c r="D44" s="2">
-        <v>-1752.8203380116399</v>
+        <v>-956.18280758865706</v>
       </c>
       <c r="E44" s="2">
-        <v>-1672.7494666477401</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-41.387478502614002</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>48</v>
       </c>
       <c r="B45" s="2">
-        <v>-73.651771942259302</v>
+        <v>149.87461028190199</v>
       </c>
       <c r="C45" s="2">
-        <v>-961.49807184222902</v>
+        <v>-788.14263853456396</v>
       </c>
       <c r="D45" s="2">
-        <v>-1825.9709002030199</v>
+        <v>-948.820402779814</v>
       </c>
       <c r="E45" s="2">
-        <v>-1697.1008658763401</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-28.256318592539301</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>49</v>
       </c>
       <c r="B46" s="2">
-        <v>-4.2903717082276698</v>
+        <v>261.73359445213902</v>
       </c>
       <c r="C46" s="2">
-        <v>-635.651347745002</v>
+        <v>-465.97810407411799</v>
       </c>
       <c r="D46" s="2">
-        <v>-1594.6549575036299</v>
+        <v>-711.54836085354202</v>
       </c>
       <c r="E46" s="2">
-        <v>-1691.4382373481999</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-20.438126940900901</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>50</v>
       </c>
       <c r="B47" s="2">
-        <v>-78.661532492984605</v>
+        <v>168.95867595619001</v>
       </c>
       <c r="C47" s="2">
-        <v>-971.993374861181</v>
+        <v>-800.25861728608595</v>
       </c>
       <c r="D47" s="2">
-        <v>-1805.97012506497</v>
+        <v>-941.99908241667299</v>
       </c>
       <c r="E47" s="2">
-        <v>-1637.32605754774</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-13.519165604746499</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B48" s="2">
-        <v>-122.201885476199</v>
+        <v>71.640733623408593</v>
       </c>
       <c r="C48" s="2">
-        <v>-944.51523927619803</v>
+        <v>-804.33779632246706</v>
       </c>
       <c r="D48" s="2">
         <v>0</v>
@@ -2154,75 +2156,75 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>52</v>
       </c>
       <c r="B49" s="2">
-        <v>2.81640493950461</v>
+        <v>236.46724907797801</v>
       </c>
       <c r="C49" s="2">
-        <v>-952.07182219689605</v>
+        <v>-802.90721924854802</v>
       </c>
       <c r="D49" s="2">
-        <v>-1595.3493537193101</v>
+        <v>-979.81204202515903</v>
       </c>
       <c r="E49" s="2">
-        <v>-1494.18232069345</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-97.426334644310202</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B50" s="2">
-        <v>-23.3884302464519</v>
+        <v>226.809094815864</v>
       </c>
       <c r="C50" s="2">
-        <v>-916.85135410355304</v>
+        <v>-760.824513382948</v>
       </c>
       <c r="D50" s="2">
-        <v>-1804.96564978387</v>
+        <v>-949.16369971767699</v>
       </c>
       <c r="E50" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>54</v>
       </c>
       <c r="B51" s="2">
-        <v>14.144686245712601</v>
+        <v>160.03086505180201</v>
       </c>
       <c r="C51" s="2">
-        <v>-965.41188262732203</v>
+        <v>-796.35061699763799</v>
       </c>
       <c r="D51" s="2">
-        <v>-1822.5958525916501</v>
+        <v>-942.65088940820999</v>
       </c>
       <c r="E51" s="2">
-        <v>-1476.75163059796</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.02035020654625</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B52" s="2">
-        <v>-105.65103978125001</v>
+        <v>138.25735023127601</v>
       </c>
       <c r="C52" s="2">
-        <v>-958.57844905915499</v>
+        <v>-793.50012086782101</v>
       </c>
       <c r="D52" s="2">
-        <v>-1811.20755985085</v>
+        <v>-941.079828071409</v>
       </c>
       <c r="E52" s="2">
-        <v>-1632.45991435172</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-61.029129602323202</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>56</v>
       </c>
@@ -2230,33 +2232,33 @@
         <v>0</v>
       </c>
       <c r="C53" s="2">
-        <v>-894.26703954127299</v>
+        <v>-726.34857416915202</v>
       </c>
       <c r="D53" s="2">
-        <v>-1795.31193427075</v>
+        <v>-932.39735058774204</v>
       </c>
       <c r="E53" s="2">
-        <v>-1680.21534989474</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-6.3878293868613101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>57</v>
       </c>
       <c r="B54" s="2">
-        <v>13.676569062275</v>
+        <v>285.479382821591</v>
       </c>
       <c r="C54" s="2">
-        <v>-937.32214279200196</v>
+        <v>-761.730608978296</v>
       </c>
       <c r="D54" s="2">
-        <v>-1655.62936608672</v>
+        <v>-804.27859974015905</v>
       </c>
       <c r="E54" s="2">
-        <v>-1547.12656800888</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-12.5316525164437</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>58</v>
       </c>
@@ -2267,81 +2269,81 @@
         <v>0</v>
       </c>
       <c r="D55" s="2">
-        <v>-1805.9951414689299</v>
+        <v>-928.3701598737</v>
       </c>
       <c r="E55" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>59</v>
       </c>
       <c r="B56" s="2">
-        <v>-78.154968696770496</v>
+        <v>123.49128771081899</v>
       </c>
       <c r="C56" s="2">
-        <v>-983.24918522522898</v>
+        <v>-815.77306892623596</v>
       </c>
       <c r="D56" s="2">
-        <v>-1844.06245075329</v>
+        <v>-954.87717783343396</v>
       </c>
       <c r="E56" s="2">
-        <v>-1658.3618521303699</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-13.0839774808911</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>60</v>
       </c>
       <c r="B57" s="2">
-        <v>-75.306583961309101</v>
+        <v>185.130252649618</v>
       </c>
       <c r="C57" s="2">
-        <v>-975.01072467731103</v>
+        <v>-805.05915925899001</v>
       </c>
       <c r="D57" s="2">
-        <v>-1821.0760378397099</v>
+        <v>-928.19463189848102</v>
       </c>
       <c r="E57" s="2">
-        <v>-1687.28455529024</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-0.14488118725207499</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>61</v>
       </c>
       <c r="B58" s="2">
-        <v>-20.416469959506099</v>
+        <v>212.05952626180201</v>
       </c>
       <c r="C58" s="2">
         <v>0</v>
       </c>
       <c r="D58" s="2">
-        <v>-1694.8331927663</v>
+        <v>-876.23732216700103</v>
       </c>
       <c r="E58" s="2">
-        <v>-1594.8883787925599</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.9467840572583599</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>62</v>
       </c>
       <c r="B59" s="2">
-        <v>-34.179042792687298</v>
+        <v>223.847847243204</v>
       </c>
       <c r="C59" s="2">
-        <v>-959.93053868248001</v>
+        <v>-791.40248649991895</v>
       </c>
       <c r="D59" s="2">
-        <v>-1779.95179380273</v>
+        <v>-917.27361062967702</v>
       </c>
       <c r="E59" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>63</v>
       </c>
@@ -2352,55 +2354,55 @@
         <v>0</v>
       </c>
       <c r="D60" s="2">
-        <v>-1469.50647785298</v>
+        <v>-933.37039323888598</v>
       </c>
       <c r="E60" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>64</v>
       </c>
       <c r="B61" s="2">
-        <v>-33.550877297761403</v>
+        <v>166.56084735517999</v>
       </c>
       <c r="C61" s="2">
-        <v>-967.02527296791197</v>
+        <v>-796.72513115598099</v>
       </c>
       <c r="D61" s="2">
-        <v>-1821.1480174114199</v>
+        <v>-941.20083370046905</v>
       </c>
       <c r="E61" s="2">
-        <v>-1541.0395190315101</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-2.6443640902306198</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>65</v>
       </c>
       <c r="B62" s="2">
-        <v>-68.003611556546801</v>
+        <v>204.645403635869</v>
       </c>
       <c r="C62" s="2">
-        <v>-968.35674489119401</v>
+        <v>-796.21374192781298</v>
       </c>
       <c r="D62" s="2">
-        <v>-1766.2588592429299</v>
+        <v>-893.62028049605794</v>
       </c>
       <c r="E62" s="2">
-        <v>-1633.9886774054301</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-20.948304934146801</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>66</v>
       </c>
       <c r="B63" s="2">
-        <v>-56.8516381981824</v>
+        <v>190.39139520372501</v>
       </c>
       <c r="C63" s="2">
-        <v>-955.10733170851495</v>
+        <v>-788.781202957235</v>
       </c>
       <c r="D63" s="2">
         <v>0</v>
@@ -2409,29 +2411,29 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>67</v>
       </c>
       <c r="B64" s="2">
-        <v>-80.506657591110198</v>
+        <v>167.494231685616</v>
       </c>
       <c r="C64" s="2">
-        <v>-896.34893274513195</v>
+        <v>-771.07562494088404</v>
       </c>
       <c r="D64" s="2">
-        <v>-1756.7803616230401</v>
+        <v>-920.23295272941095</v>
       </c>
       <c r="E64" s="2">
-        <v>-1616.4395143701699</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-12.717770822023001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>68</v>
       </c>
       <c r="B65" s="2">
-        <v>-15.1152027240846</v>
+        <v>240.39849554703801</v>
       </c>
       <c r="C65" s="2">
         <v>0</v>
@@ -2440,44 +2442,44 @@
         <v>0</v>
       </c>
       <c r="E65" s="2">
-        <v>-1667.3960375900499</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+        <v>9.2001969458586395</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>69</v>
       </c>
       <c r="B66" s="2">
-        <v>-86.196662521621903</v>
+        <v>173.42487832932099</v>
       </c>
       <c r="C66" s="2">
         <v>0</v>
       </c>
       <c r="D66" s="2">
-        <v>-1313.1623829085399</v>
+        <v>-455.13315068462202</v>
       </c>
       <c r="E66" s="2">
-        <v>-1725.1750194882</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-50.044178707346902</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>70</v>
       </c>
       <c r="B67" s="2">
-        <v>-62.528658552305103</v>
+        <v>119.978953729145</v>
       </c>
       <c r="C67" s="2">
-        <v>-923.71807737706604</v>
+        <v>-807.33360400936203</v>
       </c>
       <c r="D67" s="2">
-        <v>-1851.29730026213</v>
+        <v>-966.94043632536898</v>
       </c>
       <c r="E67" s="2">
-        <v>-1576.8296814277101</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-7.7438252769157403</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>71</v>
       </c>
@@ -2491,61 +2493,61 @@
         <v>0</v>
       </c>
       <c r="E68" s="2">
-        <v>-1667.31527983007</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-6.0949733436179896</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>72</v>
       </c>
       <c r="B69" s="2">
-        <v>-24.434269579181802</v>
+        <v>246.34060123967299</v>
       </c>
       <c r="C69" s="2">
-        <v>-905.41357469328204</v>
+        <v>-751.60986912276098</v>
       </c>
       <c r="D69" s="2">
-        <v>-1793.2376495405899</v>
+        <v>-901.95179690763302</v>
       </c>
       <c r="E69" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>73</v>
       </c>
       <c r="B70" s="2">
-        <v>4.6972514316478904</v>
+        <v>267.29750086710101</v>
       </c>
       <c r="C70" s="2">
-        <v>-899.11467631808205</v>
+        <v>-741.52661999991301</v>
       </c>
       <c r="D70" s="2">
-        <v>-1770.25563552125</v>
+        <v>-897.81230483276499</v>
       </c>
       <c r="E70" s="2">
-        <v>-1676.31437582849</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-0.95940373475559704</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>74</v>
       </c>
       <c r="B71" s="2">
-        <v>-216.31670685463999</v>
+        <v>-64.419591451528504</v>
       </c>
       <c r="C71" s="2">
-        <v>-354.20804322057597</v>
+        <v>-271.84642241281301</v>
       </c>
       <c r="D71" s="2">
-        <v>-1282.15991508662</v>
+        <v>-492.87159765638199</v>
       </c>
       <c r="E71" s="2">
-        <v>-1767.5510558705701</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-192.32715006449999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>75</v>
       </c>
@@ -2553,84 +2555,84 @@
         <v>0</v>
       </c>
       <c r="C72" s="2">
-        <v>-692.33149865597704</v>
+        <v>-525.14280310257095</v>
       </c>
       <c r="D72" s="2">
-        <v>-1567.23946221079</v>
+        <v>-677.71402626719805</v>
       </c>
       <c r="E72" s="2">
-        <v>-1665.70155170975</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+        <v>10.5138453337977</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B73" s="2">
-        <v>17.269386427410801</v>
+        <v>281.39350646974401</v>
       </c>
       <c r="C73" s="2">
-        <v>-868.78688598926306</v>
+        <v>-700.23190103671698</v>
       </c>
       <c r="D73" s="2">
-        <v>-1689.64686583364</v>
+        <v>-866.14467737305597</v>
       </c>
       <c r="E73" s="2">
-        <v>-1675.07011191674</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-9.8084737755048099</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>77</v>
       </c>
       <c r="B74" s="2">
-        <v>21.342849366650199</v>
+        <v>287.86254762570599</v>
       </c>
       <c r="C74" s="2">
-        <v>-843.018586562991</v>
+        <v>-672.27844664624695</v>
       </c>
       <c r="D74" s="2">
-        <v>-1760.02073647527</v>
+        <v>-877.22826594141202</v>
       </c>
       <c r="E74" s="2">
-        <v>-1648.8074990943301</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+        <v>21.124681677690202</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>78</v>
       </c>
       <c r="B75" s="2">
-        <v>25.600143398876799</v>
+        <v>288.40490324616098</v>
       </c>
       <c r="C75" s="2">
-        <v>-724.59001229306102</v>
+        <v>-584.47786412695405</v>
       </c>
       <c r="D75" s="2">
-        <v>-1437.5301518024501</v>
+        <v>-627.34227613862402</v>
       </c>
       <c r="E75" s="2">
-        <v>-1706.37250735579</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-8.3918387941143902</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>79</v>
       </c>
       <c r="B76" s="2">
-        <v>34.197692143290404</v>
+        <v>294.60494988684701</v>
       </c>
       <c r="C76" s="2">
-        <v>-858.083918803507</v>
+        <v>-714.16911229580501</v>
       </c>
       <c r="D76" s="2">
-        <v>-1470.95893531251</v>
+        <v>-684.56501832383105</v>
       </c>
       <c r="E76" s="2">
-        <v>-1588.3483991103799</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+        <v>14.596520712041199</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>80</v>
       </c>
@@ -2647,58 +2649,58 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>81</v>
       </c>
       <c r="B78" s="2">
-        <v>-83.809392409176496</v>
+        <v>158.558999656759</v>
       </c>
       <c r="C78" s="2">
-        <v>-937.29966186569698</v>
+        <v>-766.93936475259602</v>
       </c>
       <c r="D78" s="2">
-        <v>-1826.45445213165</v>
+        <v>-936.61846057834998</v>
       </c>
       <c r="E78" s="2">
-        <v>-1683.1263283405699</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+        <v>4.0052697478998898</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>82</v>
       </c>
       <c r="B79" s="2">
-        <v>-6.3056196534903401</v>
+        <v>262.397410424584</v>
       </c>
       <c r="C79" s="2">
-        <v>-966.97365648734399</v>
+        <v>-797.22018497658701</v>
       </c>
       <c r="D79" s="2">
-        <v>-1670.6618218928299</v>
+        <v>-805.33818527524397</v>
       </c>
       <c r="E79" s="2">
-        <v>-1642.14332151386</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+        <v>3.9533154504558801</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>83</v>
       </c>
       <c r="B80" s="2">
-        <v>50.750733617729402</v>
+        <v>219.58711168516399</v>
       </c>
       <c r="C80" s="2">
-        <v>-891.67413035328002</v>
+        <v>-804.23610851209901</v>
       </c>
       <c r="D80" s="2">
-        <v>-1779.13082771428</v>
+        <v>-953.36223974186805</v>
       </c>
       <c r="E80" s="2">
-        <v>-1440.8181994614199</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-3.37849938402523</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>84</v>
       </c>
@@ -2706,106 +2708,106 @@
         <v>0</v>
       </c>
       <c r="C81" s="2">
-        <v>-957.62602634297798</v>
+        <v>-787.826857466962</v>
       </c>
       <c r="D81" s="2">
-        <v>-1768.2548939542901</v>
+        <v>-949.89468114756096</v>
       </c>
       <c r="E81" s="2">
-        <v>-1684.0232878859799</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-26.9711953127157</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B82" s="2">
-        <v>-53.244179163678403</v>
+        <v>209.481893208874</v>
       </c>
       <c r="C82" s="2">
-        <v>-939.12133958760603</v>
+        <v>-774.32080125121001</v>
       </c>
       <c r="D82" s="2">
-        <v>-1766.7051766381101</v>
+        <v>-889.15648219090997</v>
       </c>
       <c r="E82" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>86</v>
       </c>
       <c r="B83" s="2">
-        <v>-4.6293536797933301</v>
+        <v>262.03055764371601</v>
       </c>
       <c r="C83" s="2">
-        <v>-910.06980558563998</v>
+        <v>-736.01205906693394</v>
       </c>
       <c r="D83" s="2">
-        <v>-1778.0795132390399</v>
+        <v>-888.23598119656299</v>
       </c>
       <c r="E83" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>87</v>
       </c>
       <c r="B84" s="2">
-        <v>-11.733310407976299</v>
+        <v>228.57028099266199</v>
       </c>
       <c r="C84" s="2">
-        <v>-967.12291210117201</v>
+        <v>-799.53714330818502</v>
       </c>
       <c r="D84" s="2">
-        <v>-1657.9130139123399</v>
+        <v>-962.626943056247</v>
       </c>
       <c r="E84" s="2">
-        <v>-1681.1720735742899</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-40.380191763274098</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B85" s="2">
-        <v>10.991543883670101</v>
+        <v>280.765154496278</v>
       </c>
       <c r="C85" s="2">
-        <v>-869.88311582018605</v>
+        <v>-709.09020823569801</v>
       </c>
       <c r="D85" s="2">
-        <v>-1644.93061939209</v>
+        <v>-852.91054051498304</v>
       </c>
       <c r="E85" s="2">
-        <v>-1690.1034261223101</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1.53070197804243</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B86" s="2">
-        <v>5.0279996531779201</v>
+        <v>267.73486833913898</v>
       </c>
       <c r="C86" s="2">
         <v>0</v>
       </c>
       <c r="D86" s="2">
-        <v>-1807.54595895324</v>
+        <v>-932.945686718204</v>
       </c>
       <c r="E86" s="2">
-        <v>-1673.1742935099401</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-30.895766288550799</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>90</v>
       </c>
       <c r="B87" s="2">
-        <v>4.9044898918988098</v>
+        <v>219.26841060759901</v>
       </c>
       <c r="C87" s="2">
         <v>0</v>
@@ -2814,78 +2816,78 @@
         <v>0</v>
       </c>
       <c r="E87" s="2">
-        <v>-1563.5825969437001</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-12.0224220110749</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B88" s="2">
-        <v>13.4324629687091</v>
+        <v>213.02288423210399</v>
       </c>
       <c r="C88" s="2">
-        <v>-953.05154745035099</v>
+        <v>-818.83745328865905</v>
       </c>
       <c r="D88" s="2">
-        <v>-1475.31975702626</v>
+        <v>-980.80646180806798</v>
       </c>
       <c r="E88" s="2">
-        <v>-1577.54048518791</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-60.363141945090099</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>92</v>
       </c>
       <c r="B89" s="2">
-        <v>-19.963224283254601</v>
+        <v>233.48671349457601</v>
       </c>
       <c r="C89" s="2">
-        <v>-962.08626929715194</v>
+        <v>-793.18433146795098</v>
       </c>
       <c r="D89" s="2">
-        <v>-1784.12091093195</v>
+        <v>-921.87448897068998</v>
       </c>
       <c r="E89" s="2">
-        <v>-1644.69619058852</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-17.9098722721928</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>93</v>
       </c>
       <c r="B90" s="2">
-        <v>-64.929699468283303</v>
+        <v>216.10505285819301</v>
       </c>
       <c r="C90" s="2">
-        <v>-959.82585234696899</v>
+        <v>-791.41627097062099</v>
       </c>
       <c r="D90" s="2">
         <v>0</v>
       </c>
       <c r="E90" s="2">
-        <v>-1709.1436268441801</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-23.837850658194199</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B91" s="2">
-        <v>-49.581932858572898</v>
+        <v>166.14118596722599</v>
       </c>
       <c r="C91" s="2">
-        <v>-981.52096418703297</v>
+        <v>-816.61583751244802</v>
       </c>
       <c r="D91" s="2">
-        <v>-1737.15175157162</v>
+        <v>-968.45587760555895</v>
       </c>
       <c r="E91" s="2">
-        <v>-1548.6228800579599</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-74.958307782969499</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>95</v>
       </c>
@@ -2899,27 +2901,27 @@
         <v>0</v>
       </c>
       <c r="E92" s="2">
-        <v>-1591.1172152207</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-3.8464398369876598</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>96</v>
       </c>
       <c r="B93" s="2">
-        <v>-21.828198117577401</v>
+        <v>244.443800458053</v>
       </c>
       <c r="C93" s="2">
-        <v>-630.11133161542</v>
+        <v>-482.48983156211</v>
       </c>
       <c r="D93" s="2">
         <v>0</v>
       </c>
       <c r="E93" s="2">
-        <v>-1656.64656523952</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+        <v>20.891337123564899</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>97</v>
       </c>
@@ -2927,16 +2929,16 @@
         <v>0</v>
       </c>
       <c r="C94" s="2">
-        <v>-872.83722461945695</v>
+        <v>-714.06016701993406</v>
       </c>
       <c r="D94" s="2">
-        <v>-1809.1796700431901</v>
+        <v>-925.58417802265399</v>
       </c>
       <c r="E94" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>98</v>
       </c>
@@ -2944,7 +2946,7 @@
         <v>0</v>
       </c>
       <c r="C95" s="2">
-        <v>-684.08385139137897</v>
+        <v>-510.89457341779001</v>
       </c>
       <c r="D95" s="2">
         <v>0</v>
@@ -2953,97 +2955,97 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>99</v>
       </c>
       <c r="B96" s="2">
-        <v>-18.046573957987199</v>
+        <v>246.21762726890699</v>
       </c>
       <c r="C96" s="2">
-        <v>-957.75024004055604</v>
+        <v>-790.02137314357901</v>
       </c>
       <c r="D96" s="2">
-        <v>-1819.74555434383</v>
+        <v>-937.46710512272398</v>
       </c>
       <c r="E96" s="2">
-        <v>-1688.2461380468401</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-8.5720043708004408</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>100</v>
       </c>
       <c r="B97" s="2">
-        <v>-49.991033591581399</v>
+        <v>-26.015545722956102</v>
       </c>
       <c r="C97" s="2">
-        <v>-1000.32800325165</v>
+        <v>-941.29589832287195</v>
       </c>
       <c r="D97" s="2">
-        <v>-1826.4487962068599</v>
+        <v>-1058.85498445751</v>
       </c>
       <c r="E97" s="2">
-        <v>-1460.2529072059399</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-116.980002493927</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>101</v>
       </c>
       <c r="B98" s="2">
-        <v>-5.67861865065984</v>
+        <v>224.29674981694799</v>
       </c>
       <c r="C98" s="2">
-        <v>-922.62713114530004</v>
+        <v>-786.81889500209695</v>
       </c>
       <c r="D98" s="2">
-        <v>-1783.3428891651899</v>
+        <v>-944.233751162918</v>
       </c>
       <c r="E98" s="2">
-        <v>-1565.1169582084301</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-8.7744427378293697</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>102</v>
       </c>
       <c r="B99" s="2">
-        <v>-65.107941620862206</v>
+        <v>191.15964606962899</v>
       </c>
       <c r="C99" s="2">
-        <v>-855.87399935141195</v>
+        <v>-678.61157437652605</v>
       </c>
       <c r="D99" s="2">
-        <v>-1452.24045706727</v>
+        <v>-575.37154830517602</v>
       </c>
       <c r="E99" s="2">
-        <v>-1736.19547301578</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-57.589848643787299</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>103</v>
       </c>
       <c r="B100" s="2">
-        <v>-42.730620602048702</v>
+        <v>225.89844908834499</v>
       </c>
       <c r="C100" s="2">
-        <v>-966.67307690033897</v>
+        <v>-791.53252756476297</v>
       </c>
       <c r="D100" s="2">
-        <v>-1696.7337570080699</v>
+        <v>-813.65517862747004</v>
       </c>
       <c r="E100" s="2">
-        <v>-1745.69180488558</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-66.371626187231001</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>104</v>
       </c>
       <c r="B101" s="2">
-        <v>-134.276163779575</v>
+        <v>136.62434732068499</v>
       </c>
       <c r="C101" s="2">
         <v>0</v>
@@ -3052,69 +3054,69 @@
         <v>0</v>
       </c>
       <c r="E101" s="2">
-        <v>-1644.65232964906</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-14.460513852365899</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>105</v>
       </c>
       <c r="B102" s="2">
-        <v>-19.324485699248999</v>
+        <v>202.070267692014</v>
       </c>
       <c r="C102" s="2">
-        <v>-975.78359236455503</v>
+        <v>-804.97760640379704</v>
       </c>
       <c r="D102" s="2">
-        <v>-1823.60324369821</v>
+        <v>-946.65125433833396</v>
       </c>
       <c r="E102" s="2">
-        <v>-1682.1399209495701</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-2.6555782099081</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>106</v>
       </c>
       <c r="B103" s="2">
-        <v>-16.320855907915998</v>
+        <v>184.64545896691399</v>
       </c>
       <c r="C103" s="2">
-        <v>-933.07569780554797</v>
+        <v>-790.64698644149303</v>
       </c>
       <c r="D103" s="2">
-        <v>-1817.7939674642801</v>
+        <v>-943.77392360407202</v>
       </c>
       <c r="E103" s="2">
-        <v>-1591.6160379681801</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+        <v>3.3836035291247999</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>107</v>
       </c>
       <c r="B104" s="2">
-        <v>-9.7265333598059005</v>
+        <v>254.55432318550601</v>
       </c>
       <c r="C104" s="2">
-        <v>-847.03358622765404</v>
+        <v>-670.48054837376696</v>
       </c>
       <c r="D104" s="2">
-        <v>-1486.85996772109</v>
+        <v>-588.356744814065</v>
       </c>
       <c r="E104" s="2">
-        <v>-1689.4538706717599</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-18.352766076788601</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>108</v>
       </c>
       <c r="B105" s="2">
-        <v>-49.703588062706103</v>
+        <v>221.20054199462299</v>
       </c>
       <c r="C105" s="2">
-        <v>-934.44412342002101</v>
+        <v>-765.43048381459801</v>
       </c>
       <c r="D105" s="2">
         <v>0</v>
@@ -3123,12 +3125,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>109</v>
       </c>
       <c r="B106" s="2">
-        <v>-87.075660277109705</v>
+        <v>158.848149289177</v>
       </c>
       <c r="C106" s="2">
         <v>0</v>
@@ -3140,92 +3142,92 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>110</v>
       </c>
       <c r="B107" s="2">
-        <v>-32.051849812232298</v>
+        <v>213.28533366565199</v>
       </c>
       <c r="C107" s="2">
-        <v>-951.61985503788196</v>
+        <v>-785.28622518142697</v>
       </c>
       <c r="D107" s="2">
         <v>0</v>
       </c>
       <c r="E107" s="2">
-        <v>-1675.8488984309299</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1.7921250512042699</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>111</v>
       </c>
       <c r="B108" s="2">
-        <v>-13.603435221264601</v>
+        <v>250.99793731558799</v>
       </c>
       <c r="C108" s="2">
-        <v>-633.29699508128704</v>
+        <v>-467.05538760254899</v>
       </c>
       <c r="D108" s="2">
-        <v>-1514.62379341782</v>
+        <v>-626.92178394432494</v>
       </c>
       <c r="E108" s="2">
-        <v>-1679.91950301612</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-7.3556695769984799</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B109" s="2">
-        <v>-28.6789201214015</v>
+        <v>178.493774093703</v>
       </c>
       <c r="C109" s="2">
-        <v>-973.52505274887505</v>
+        <v>-802.16707698044604</v>
       </c>
       <c r="D109" s="2">
-        <v>-1799.0105828788201</v>
+        <v>-943.26298670387905</v>
       </c>
       <c r="E109" s="2">
-        <v>-1647.07544419533</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-39.068140942788901</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>113</v>
       </c>
       <c r="B110" s="2">
-        <v>-40.327705666284402</v>
+        <v>164.50011968139501</v>
       </c>
       <c r="C110" s="2">
-        <v>-912.36712424352004</v>
+        <v>-771.86130150375095</v>
       </c>
       <c r="D110" s="2">
-        <v>-1810.5694964132199</v>
+        <v>-944.69683411839799</v>
       </c>
       <c r="E110" s="2">
-        <v>-1686.67786466866</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-5.0281961756961699</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>114</v>
       </c>
       <c r="B111" s="2">
-        <v>-43.208563066971003</v>
+        <v>158.335165906366</v>
       </c>
       <c r="C111" s="2">
-        <v>-834.70597531280396</v>
+        <v>-700.86081034466201</v>
       </c>
       <c r="D111" s="2">
-        <v>-1829.3085153674899</v>
+        <v>-943.84177677190405</v>
       </c>
       <c r="E111" s="2">
-        <v>-1661.7891397130199</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-5.0785029645428503</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>115</v>
       </c>
@@ -3233,50 +3235,50 @@
         <v>0</v>
       </c>
       <c r="C112" s="2">
-        <v>-966.56143578401498</v>
+        <v>-811.07110799504096</v>
       </c>
       <c r="D112" s="2">
-        <v>-1627.3350709699</v>
+        <v>-998.54910502164103</v>
       </c>
       <c r="E112" s="2">
-        <v>-1711.09099554404</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-94.155944171623105</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>116</v>
       </c>
       <c r="B113" s="2">
-        <v>-100.328603128634</v>
+        <v>170.26444540087101</v>
       </c>
       <c r="C113" s="2">
-        <v>-942.04000076520197</v>
+        <v>-772.38615094800002</v>
       </c>
       <c r="D113" s="2">
-        <v>-1824.33371303987</v>
+        <v>-942.36399448129498</v>
       </c>
       <c r="E113" s="2">
-        <v>-1698.18482044192</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-17.401335788110799</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>117</v>
       </c>
       <c r="B114" s="2">
-        <v>-38.886676022166597</v>
+        <v>218.474347243121</v>
       </c>
       <c r="C114" s="2">
-        <v>-972.47412862917304</v>
+        <v>-806.79444562860601</v>
       </c>
       <c r="D114" s="2">
-        <v>-1809.1156498979799</v>
+        <v>-931.01741512650904</v>
       </c>
       <c r="E114" s="2">
-        <v>-1667.10127855051</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-11.356079284048599</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>118</v>
       </c>
@@ -3287,30 +3289,30 @@
         <v>0</v>
       </c>
       <c r="D115" s="2">
-        <v>-1524.61242604923</v>
+        <v>-836.32260021372599</v>
       </c>
       <c r="E115" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>119</v>
       </c>
       <c r="B116" s="2">
-        <v>-76.175776558368597</v>
+        <v>189.846482674356</v>
       </c>
       <c r="C116" s="2">
-        <v>-965.89781823338001</v>
+        <v>-794.16644338038998</v>
       </c>
       <c r="D116" s="2">
-        <v>-1813.1252691785101</v>
+        <v>-928.28260957226303</v>
       </c>
       <c r="E116" s="2">
-        <v>-1695.8891414898701</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-8.8659048725087395</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>120</v>
       </c>
@@ -3324,61 +3326,61 @@
         <v>0</v>
       </c>
       <c r="E117" s="2">
-        <v>-1673.34159882426</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+        <v>3.8061505258231101</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>121</v>
       </c>
       <c r="B118" s="2">
-        <v>11.2788396125465</v>
+        <v>234.13251692440099</v>
       </c>
       <c r="C118" s="2">
-        <v>-958.80691057972103</v>
+        <v>-789.174160554325</v>
       </c>
       <c r="D118" s="2">
-        <v>-1762.71323671602</v>
+        <v>-928.40613244636199</v>
       </c>
       <c r="E118" s="2">
-        <v>-1489.68957335096</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-19.030855341296601</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>122</v>
       </c>
       <c r="B119" s="2">
-        <v>-6.3173952342382202</v>
+        <v>221.505939385852</v>
       </c>
       <c r="C119" s="2">
-        <v>-970.92789436915496</v>
+        <v>-799.539469582283</v>
       </c>
       <c r="D119" s="2">
-        <v>-1791.7436643946501</v>
+        <v>-944.92101026859405</v>
       </c>
       <c r="E119" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>123</v>
       </c>
       <c r="B120" s="2">
-        <v>21.8387172667904</v>
+        <v>295.14185853060599</v>
       </c>
       <c r="C120" s="2">
-        <v>-674.67880940033501</v>
+        <v>-536.34710483531603</v>
       </c>
       <c r="D120" s="2">
-        <v>-1534.63527891637</v>
+        <v>-668.79867816046101</v>
       </c>
       <c r="E120" s="2">
-        <v>-1660.9363064689901</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+        <v>9.4457915555049095</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>124</v>
       </c>
@@ -3392,27 +3394,27 @@
         <v>0</v>
       </c>
       <c r="E121" s="2">
-        <v>-1505.23868706604</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-24.674781764060501</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>125</v>
       </c>
       <c r="B122" s="2">
-        <v>-29.899161864475801</v>
+        <v>186.16114852737601</v>
       </c>
       <c r="C122" s="2">
-        <v>-934.05584863878403</v>
+        <v>-777.61339560249098</v>
       </c>
       <c r="D122" s="2">
-        <v>-1827.6991045247401</v>
+        <v>-942.34085433341897</v>
       </c>
       <c r="E122" s="2">
-        <v>-1656.1850741058299</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+        <v>5.5870440155589698</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>126</v>
       </c>
@@ -3423,132 +3425,132 @@
         <v>0</v>
       </c>
       <c r="D123" s="2">
-        <v>-1743.11960872123</v>
+        <v>-903.10219108519595</v>
       </c>
       <c r="E123" s="2">
-        <v>-1491.7330119257099</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-17.449030963155401</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>127</v>
       </c>
       <c r="B124" s="2">
-        <v>-82.315317801860203</v>
+        <v>99.612281756528105</v>
       </c>
       <c r="C124" s="2">
-        <v>-899.301719801216</v>
+        <v>-794.25042514522397</v>
       </c>
       <c r="D124" s="2">
-        <v>-1814.26076233617</v>
+        <v>-944.63976997559803</v>
       </c>
       <c r="E124" s="2">
-        <v>-1472.93396121654</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-8.6018586183508905</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>128</v>
       </c>
       <c r="B125" s="2">
-        <v>-12.2093684915806</v>
+        <v>242.95919766922199</v>
       </c>
       <c r="C125" s="2">
         <v>0</v>
       </c>
       <c r="D125" s="2">
-        <v>-1802.0586931781399</v>
+        <v>-942.29477023035099</v>
       </c>
       <c r="E125" s="2">
-        <v>-1620.5531137944399</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-30.020137154023502</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>129</v>
       </c>
       <c r="B126" s="2">
-        <v>-38.892926110388103</v>
+        <v>220.679496954331</v>
       </c>
       <c r="C126" s="2">
-        <v>-941.61517660100799</v>
+        <v>-771.62911756866799</v>
       </c>
       <c r="D126" s="2">
         <v>0</v>
       </c>
       <c r="E126" s="2">
-        <v>-1681.5669222720501</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-3.0915827469870298</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>130</v>
       </c>
       <c r="B127" s="2">
-        <v>5.9687820043876902</v>
+        <v>259.21333681733603</v>
       </c>
       <c r="C127" s="2">
-        <v>-978.14910858342796</v>
+        <v>-807.68096048464099</v>
       </c>
       <c r="D127" s="2">
-        <v>-1805.8884136762599</v>
+        <v>-935.54996591995496</v>
       </c>
       <c r="E127" s="2">
-        <v>-1679.0250178828801</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-8.4240760052825294</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>131</v>
       </c>
       <c r="B128" s="2">
-        <v>25.427988677237401</v>
+        <v>293.42406403201801</v>
       </c>
       <c r="C128" s="2">
-        <v>-797.86523754099505</v>
+        <v>-619.52508189025696</v>
       </c>
       <c r="D128" s="2">
-        <v>-1559.0122027678501</v>
+        <v>-702.62140008548704</v>
       </c>
       <c r="E128" s="2">
-        <v>-1692.68861986251</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-30.278637389106699</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>132</v>
       </c>
       <c r="B129" s="2">
-        <v>14.1115002244766</v>
+        <v>273.10086053772602</v>
       </c>
       <c r="C129" s="2">
-        <v>-904.69621961359496</v>
+        <v>-742.16599306672902</v>
       </c>
       <c r="D129" s="2">
-        <v>-1712.3754410664801</v>
+        <v>-861.27454458045702</v>
       </c>
       <c r="E129" s="2">
-        <v>-1558.5268307041299</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+        <v>7.2602449783757903</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>133</v>
       </c>
       <c r="B130" s="2">
-        <v>13.0343576823647</v>
+        <v>281.13871054306202</v>
       </c>
       <c r="C130" s="2">
-        <v>-906.00388000354997</v>
+        <v>-732.995762145821</v>
       </c>
       <c r="D130" s="2">
-        <v>-1671.71002585474</v>
+        <v>-802.82570933790703</v>
       </c>
       <c r="E130" s="2">
-        <v>-1622.0367014866799</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+        <v>6.26534939033525</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>134</v>
       </c>
@@ -3556,135 +3558,135 @@
         <v>0</v>
       </c>
       <c r="C131" s="2">
-        <v>-927.59123676993499</v>
+        <v>-769.42894470338899</v>
       </c>
       <c r="D131" s="2">
-        <v>-1605.0139156066</v>
+        <v>-797.43561815915405</v>
       </c>
       <c r="E131" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>135</v>
       </c>
       <c r="B132" s="2">
-        <v>-70.728715525319203</v>
+        <v>189.84890827532899</v>
       </c>
       <c r="C132" s="2">
-        <v>-956.89453385007096</v>
+        <v>-793.54318927903898</v>
       </c>
       <c r="D132" s="2">
-        <v>-1813.29686890738</v>
+        <v>-943.54112513642895</v>
       </c>
       <c r="E132" s="2">
-        <v>-1712.62916237168</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-51.215220040582402</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>136</v>
       </c>
       <c r="B133" s="2">
-        <v>-57.245244300315903</v>
+        <v>195.29436521338101</v>
       </c>
       <c r="C133" s="2">
-        <v>-958.12944655637205</v>
+        <v>-793.39956007170201</v>
       </c>
       <c r="D133" s="2">
         <v>0</v>
       </c>
       <c r="E133" s="2">
-        <v>-1656.48351612174</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-51.919176710843601</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>137</v>
       </c>
       <c r="B134" s="2">
-        <v>-89.684432225447395</v>
+        <v>173.60930602947801</v>
       </c>
       <c r="C134" s="2">
-        <v>-431.80147497022301</v>
+        <v>-326.56803651924997</v>
       </c>
       <c r="D134" s="2">
-        <v>-1176.0148746050299</v>
+        <v>-450.64568559455802</v>
       </c>
       <c r="E134" s="2">
-        <v>-1650.49100317283</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+        <v>17.102521674282801</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>138</v>
       </c>
       <c r="B135" s="2">
-        <v>12.6427872045681</v>
+        <v>278.30000323623301</v>
       </c>
       <c r="C135" s="2">
-        <v>-825.681611850683</v>
+        <v>-667.40439259356003</v>
       </c>
       <c r="D135" s="2">
-        <v>-1660.0409037572299</v>
+        <v>-861.20534888071495</v>
       </c>
       <c r="E135" s="2">
-        <v>-1666.5032200416999</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+        <v>17.1613552639324</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>139</v>
       </c>
       <c r="B136" s="2">
-        <v>-4.0212554439750603</v>
+        <v>263.04481392846702</v>
       </c>
       <c r="C136" s="2">
-        <v>-959.075208999506</v>
+        <v>-791.53630495884795</v>
       </c>
       <c r="D136" s="2">
-        <v>-1730.81686365719</v>
+        <v>-844.18448238388896</v>
       </c>
       <c r="E136" s="2">
-        <v>-1667.3402915793499</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+        <v>8.3616381340286807</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>140</v>
       </c>
       <c r="B137" s="2">
-        <v>-35.806819192300601</v>
+        <v>223.04785857353099</v>
       </c>
       <c r="C137" s="2">
-        <v>-965.55438247825998</v>
+        <v>-796.53298744456299</v>
       </c>
       <c r="D137" s="2">
-        <v>-1823.8905310154801</v>
+        <v>-948.52616103461696</v>
       </c>
       <c r="E137" s="2">
-        <v>-1658.6533344347899</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-5.3139836437819703</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>141</v>
       </c>
       <c r="B138" s="2">
-        <v>21.178712516945598</v>
+        <v>288.61521260377702</v>
       </c>
       <c r="C138" s="2">
-        <v>-840.759617795503</v>
+        <v>-667.37041226804502</v>
       </c>
       <c r="D138" s="2">
-        <v>-1741.1690494337399</v>
+        <v>-848.58024610833195</v>
       </c>
       <c r="E138" s="2">
-        <v>-1692.69370187923</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-28.252106645024899</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
         <v>142</v>
       </c>
@@ -3701,7 +3703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="2" t="s">
         <v>143</v>
       </c>
@@ -3709,7 +3711,7 @@
         <v>0</v>
       </c>
       <c r="C140" s="2">
-        <v>-955.15811269772701</v>
+        <v>-787.76497345016901</v>
       </c>
       <c r="D140" s="2">
         <v>0</v>
@@ -3718,109 +3720,109 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>144</v>
       </c>
       <c r="B141" s="2">
-        <v>-37.587714098439399</v>
+        <v>208.33353442657301</v>
       </c>
       <c r="C141" s="2">
-        <v>-966.64935169233104</v>
+        <v>-799.03997883429997</v>
       </c>
       <c r="D141" s="2">
-        <v>-1787.6442831024599</v>
+        <v>-952.97253419373703</v>
       </c>
       <c r="E141" s="2">
-        <v>-1524.81738448086</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-43.6952955556701</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>145</v>
       </c>
       <c r="B142" s="2">
-        <v>27.7457297478139</v>
+        <v>220.54553970536301</v>
       </c>
       <c r="C142" s="2">
-        <v>-917.15583846437903</v>
+        <v>-782.40329984763503</v>
       </c>
       <c r="D142" s="2">
-        <v>-1721.38765690163</v>
+        <v>-951.21913691926898</v>
       </c>
       <c r="E142" s="2">
-        <v>-1523.77487414857</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-54.419809969530903</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="2" t="s">
         <v>146</v>
       </c>
       <c r="B143" s="2">
-        <v>-62.454102020546799</v>
+        <v>141.121170984489</v>
       </c>
       <c r="C143" s="2">
-        <v>-959.71915277689595</v>
+        <v>-800.89714695280202</v>
       </c>
       <c r="D143" s="2">
-        <v>-1774.79579468309</v>
+        <v>-921.84941825515205</v>
       </c>
       <c r="E143" s="2">
-        <v>-1499.7259070489899</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-23.464059973298401</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="2" t="s">
         <v>147</v>
       </c>
       <c r="B144" s="2">
-        <v>-62.690153890653903</v>
+        <v>179.90014979883901</v>
       </c>
       <c r="C144" s="2">
-        <v>-958.18963276020997</v>
+        <v>-788.39580400745899</v>
       </c>
       <c r="D144" s="2">
-        <v>-1547.8295971007899</v>
+        <v>-960.85209700991197</v>
       </c>
       <c r="E144" s="2">
-        <v>-1802.1445668020699</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-89.184359571449903</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>148</v>
       </c>
       <c r="B145" s="2">
-        <v>-105.046337300698</v>
+        <v>137.827800686892</v>
       </c>
       <c r="C145" s="2">
-        <v>-986.79996534697898</v>
+        <v>-814.17502121921905</v>
       </c>
       <c r="D145" s="2">
-        <v>-1808.13570293366</v>
+        <v>-916.79419042844995</v>
       </c>
       <c r="E145" s="2">
-        <v>-1671.8221651200899</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+        <v>2.4760027114292602</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>149</v>
       </c>
       <c r="B146" s="2">
-        <v>-15.125301736907399</v>
+        <v>247.46865548022001</v>
       </c>
       <c r="C146" s="2">
-        <v>-944.25779668419204</v>
+        <v>-775.51308227154402</v>
       </c>
       <c r="D146" s="2">
-        <v>-1780.87989918225</v>
+        <v>-923.81315258998995</v>
       </c>
       <c r="E146" s="2">
-        <v>-1605.44663348362</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-23.897894539569499</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>150</v>
       </c>
@@ -3837,75 +3839,75 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>151</v>
       </c>
       <c r="B148" s="2">
-        <v>-3.5109346735850502</v>
+        <v>260.11065992226202</v>
       </c>
       <c r="C148" s="2">
-        <v>-961.62574114618701</v>
+        <v>-792.90588722132702</v>
       </c>
       <c r="D148" s="2">
-        <v>-1808.0308463778399</v>
+        <v>-953.88530284615399</v>
       </c>
       <c r="E148" s="2">
-        <v>-1755.7537110171199</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-40.877004402425001</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>152</v>
       </c>
       <c r="B149" s="2">
-        <v>-21.302113524714802</v>
+        <v>237.14042282071</v>
       </c>
       <c r="C149" s="2">
-        <v>-958.47582378305196</v>
+        <v>-790.20001943772002</v>
       </c>
       <c r="D149" s="2">
-        <v>-1725.72006785843</v>
+        <v>-957.83437218233303</v>
       </c>
       <c r="E149" s="2">
-        <v>-1814.8567127799499</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-78.282975801154393</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>153</v>
       </c>
       <c r="B150" s="2">
-        <v>8.2456498610865996</v>
+        <v>210.76945002772399</v>
       </c>
       <c r="C150" s="2">
-        <v>-896.57134651645595</v>
+        <v>-806.781181670514</v>
       </c>
       <c r="D150" s="2">
-        <v>-1733.2763335424499</v>
+        <v>-966.85969276513197</v>
       </c>
       <c r="E150" s="2">
-        <v>-1435.4986902370399</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-53.0428215857482</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>154</v>
       </c>
       <c r="B151" s="2">
-        <v>34.949409660745602</v>
+        <v>271.95360669629798</v>
       </c>
       <c r="C151" s="2">
-        <v>-965.79767576518702</v>
+        <v>-795.41564274211601</v>
       </c>
       <c r="D151" s="2">
-        <v>-1786.57129132009</v>
+        <v>-924.473082625453</v>
       </c>
       <c r="E151" s="2">
-        <v>-1483.8235046985601</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-9.2237342348525999</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>155</v>
       </c>
@@ -3919,10 +3921,10 @@
         <v>0</v>
       </c>
       <c r="E152" s="2">
-        <v>-1548.31671941595</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+        <v>-17.367436596887799</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>156</v>
       </c>
@@ -3930,10 +3932,10 @@
         <v>0</v>
       </c>
       <c r="C153" s="2">
-        <v>-626.43460377891995</v>
+        <v>-462.00804055097899</v>
       </c>
       <c r="D153" s="2">
-        <v>-1666.42942200926</v>
+        <v>-779.71002439372796</v>
       </c>
       <c r="E153" s="2">
         <v>0</v>
@@ -3956,9 +3958,9 @@
       <selection sqref="A1:E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -3975,7 +3977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -3992,7 +3994,7 @@
         <v>1.9599999999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -4009,7 +4011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -4026,7 +4028,7 @@
         <v>6.6E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.12889999999999999</v>
       </c>
@@ -4043,7 +4045,7 @@
         <v>1.2999999999999999E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.97160000000000002</v>
       </c>
@@ -4060,7 +4062,7 @@
         <v>1.1999999999999999E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
@@ -4077,7 +4079,7 @@
         <v>8.2699999999999996E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>3.3000000000000002E-2</v>
       </c>
@@ -4094,7 +4096,7 @@
         <v>0.95269999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1E-4</v>
       </c>
@@ -4111,7 +4113,7 @@
         <v>0.123</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1E-4</v>
       </c>
@@ -4128,7 +4130,7 @@
         <v>0.97570000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1.1000000000000001E-3</v>
       </c>
@@ -4145,7 +4147,7 @@
         <v>0.87180000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0.89939999999999998</v>
       </c>
@@ -4162,7 +4164,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
@@ -4179,7 +4181,7 @@
         <v>8.2900000000000001E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -4196,7 +4198,7 @@
         <v>0.53069999999999995</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0.87450000000000006</v>
       </c>
@@ -4213,7 +4215,7 @@
         <v>2.1100000000000001E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0</v>
       </c>
@@ -4230,7 +4232,7 @@
         <v>0.81510000000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1E-4</v>
       </c>
@@ -4247,7 +4249,7 @@
         <v>0.123</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>0</v>
       </c>
@@ -4264,7 +4266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0</v>
       </c>
@@ -4281,7 +4283,7 @@
         <v>6.6E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0.98629999999999995</v>
       </c>
@@ -4309,7 +4311,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>